<commit_message>
Added pseudo code for collisions
</commit_message>
<xml_diff>
--- a/Memory locations.xlsx
+++ b/Memory locations.xlsx
@@ -1,31 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colt\Documents\School\Fall 2020\ECE 3710-001\Lab\ECE3710Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\ECE3710Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0173FDEA-0220-4BCA-A11D-6217D619A5CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2F55795-581A-4CA4-AD7F-56B0F0413A39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15945" xr2:uid="{C282C4F2-5A76-426A-8497-3189F655D365}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C282C4F2-5A76-426A-8497-3189F655D365}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Memory" sheetId="1" r:id="rId1"/>
+    <sheet name="Collision Pseudo Code" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="162">
   <si>
     <t>0x0000</t>
   </si>
@@ -418,13 +428,106 @@
   </si>
   <si>
     <t>C642</t>
+  </si>
+  <si>
+    <t>Main Ship getting hit</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>Top left pixel is the x-pos of object</t>
+  </si>
+  <si>
+    <t>Collision points</t>
+  </si>
+  <si>
+    <t>get enemy bullet collision points</t>
+  </si>
+  <si>
+    <t>Check Collision top</t>
+  </si>
+  <si>
+    <t>get ship location (s_xpos)</t>
+  </si>
+  <si>
+    <t>get enemy bullet locations(b_xpos)</t>
+  </si>
+  <si>
+    <t>-&gt; top left = b_xpos+ screen_width + 3</t>
+  </si>
+  <si>
+    <t>-&gt; bottom right = b_xpos + (screen_width*6) + 4</t>
+  </si>
+  <si>
+    <t>-&gt;if (s_xpos &lt;= bottom_right &lt;= s_xpos+15)</t>
+  </si>
+  <si>
+    <t>-&gt;-&gt;Collision</t>
+  </si>
+  <si>
+    <t>Check Collision left and right</t>
+  </si>
+  <si>
+    <t>-&gt;var loc = s_xpos + screen_width</t>
+  </si>
+  <si>
+    <t>-&gt;var end = s_xpos + (screen_width*16)</t>
+  </si>
+  <si>
+    <t>-&gt;for(loc; loc &lt; end; loc + screen_width)</t>
+  </si>
+  <si>
+    <t>-&gt;-&gt;-&gt;Collision (we can break loop)</t>
+  </si>
+  <si>
+    <t>Collision main</t>
+  </si>
+  <si>
+    <t>Collision enemy</t>
+  </si>
+  <si>
+    <t>get enemy location (e_xpos)</t>
+  </si>
+  <si>
+    <t>get ship bullet locations(b_xpos)</t>
+  </si>
+  <si>
+    <t>Check Collision bottom</t>
+  </si>
+  <si>
+    <t>get ship bullet collision points</t>
+  </si>
+  <si>
+    <t>var e_bottom = e_xpos + (screen_width*15)</t>
+  </si>
+  <si>
+    <t>-&gt;if (e_bottom &lt;= top_left &lt;= e_bottom+15)</t>
+  </si>
+  <si>
+    <t>-&gt;var loc = e_bottom - screen_width</t>
+  </si>
+  <si>
+    <t>-&gt;var end = e_xpos - screen_width</t>
+  </si>
+  <si>
+    <t>-&gt;for(loc; loc &gt; end; loc - screen_width)</t>
+  </si>
+  <si>
+    <t>-&gt;-&gt;if(bottom_right == loc || top_left== loc + 15)</t>
+  </si>
+  <si>
+    <t>-&gt;-&gt;if(bottom_right == loc || top_left == loc + 15)</t>
+  </si>
+  <si>
+    <t>Enemy Ship getting hit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -438,8 +541,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="6"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <color theme="0"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -464,8 +588,68 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFB7F6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEB1DC4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF25FF49"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="60">
     <border>
       <left/>
       <right/>
@@ -535,11 +719,764 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="9"/>
+      </left>
+      <right style="thin">
+        <color theme="9"/>
+      </right>
+      <top style="thin">
+        <color theme="9"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="9"/>
+      </left>
+      <right style="thin">
+        <color theme="9"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="9"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="9"/>
+      </right>
+      <top style="thin">
+        <color theme="9"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="9"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="9"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="9"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="9"/>
+      </right>
+      <top style="thin">
+        <color theme="9"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="9"/>
+      </left>
+      <right style="thin">
+        <color theme="9"/>
+      </right>
+      <top style="thin">
+        <color theme="9"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="9"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="9"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF25FF49"/>
+      </left>
+      <right style="thin">
+        <color theme="9"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF25FF49"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="9"/>
+      </left>
+      <right style="thin">
+        <color theme="9"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF25FF49"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="9"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF25FF49"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF25FF49"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF25FF49"/>
+      </left>
+      <right style="thin">
+        <color theme="9"/>
+      </right>
+      <top style="thin">
+        <color theme="9"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="9"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF25FF49"/>
+      </right>
+      <top style="thin">
+        <color theme="9"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF25FF49"/>
+      </left>
+      <right style="thin">
+        <color theme="9"/>
+      </right>
+      <top style="thin">
+        <color theme="9"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF25FF49"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="9"/>
+      </left>
+      <right style="thin">
+        <color theme="9"/>
+      </right>
+      <top style="thin">
+        <color theme="9"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF25FF49"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="9"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF25FF49"/>
+      </right>
+      <top style="thin">
+        <color theme="9"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF25FF49"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="9"/>
+      </left>
+      <right style="thin">
+        <color theme="9"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF25FF49"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="1" diagonalDown="1">
+      <left style="medium">
+        <color rgb="FF25FF49"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFF00"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF25FF49"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFF00"/>
+      </bottom>
+      <diagonal style="thin">
+        <color rgb="FFFFFF00"/>
+      </diagonal>
+    </border>
+    <border diagonalUp="1" diagonalDown="1">
+      <left style="thin">
+        <color rgb="FFFFFF00"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFF00"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF25FF49"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFF00"/>
+      </bottom>
+      <diagonal style="thin">
+        <color rgb="FFFFFF00"/>
+      </diagonal>
+    </border>
+    <border diagonalUp="1" diagonalDown="1">
+      <left style="thin">
+        <color rgb="FFFFFF00"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFF00"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFF00"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFF00"/>
+      </bottom>
+      <diagonal style="thin">
+        <color rgb="FFFFFF00"/>
+      </diagonal>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="9"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFF00"/>
+      </right>
+      <top style="thin">
+        <color theme="9"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="9"/>
+      </left>
+      <right style="thin">
+        <color theme="9"/>
+      </right>
+      <top style="thin">
+        <color theme="9"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFF00"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="9"/>
+      </left>
+      <right style="thin">
+        <color theme="9"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF25FF49"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFF00"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="1" diagonalDown="1">
+      <left style="thin">
+        <color rgb="FFFFFF00"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF25FF49"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF25FF49"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFF00"/>
+      </bottom>
+      <diagonal style="thin">
+        <color rgb="FFFFFF00"/>
+      </diagonal>
+    </border>
+    <border diagonalUp="1" diagonalDown="1">
+      <left style="medium">
+        <color rgb="FF25FF49"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFF00"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFF00"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFF00"/>
+      </bottom>
+      <diagonal style="thin">
+        <color rgb="FFFFFF00"/>
+      </diagonal>
+    </border>
+    <border diagonalUp="1" diagonalDown="1">
+      <left style="thin">
+        <color rgb="FFFFFF00"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF25FF49"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFF00"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFF00"/>
+      </bottom>
+      <diagonal style="thin">
+        <color rgb="FFFFFF00"/>
+      </diagonal>
+    </border>
+    <border diagonalUp="1" diagonalDown="1">
+      <left style="thin">
+        <color rgb="FFFFFF00"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF25FF49"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFF00"/>
+      </top>
+      <bottom/>
+      <diagonal style="thin">
+        <color rgb="FFFFFF00"/>
+      </diagonal>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="9"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFFFF00"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="1" diagonalDown="1">
+      <left style="medium">
+        <color rgb="FF25FF49"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFF00"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFF00"/>
+      </top>
+      <bottom/>
+      <diagonal style="thin">
+        <color rgb="FFFFFF00"/>
+      </diagonal>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="9"/>
+      </left>
+      <right style="thin">
+        <color theme="9"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="1" diagonalDown="1">
+      <left style="medium">
+        <color rgb="FF25FF49"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFF00"/>
+      </right>
+      <top style="thin">
+        <color theme="9"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF25FF49"/>
+      </bottom>
+      <diagonal style="thin">
+        <color rgb="FFFFFF00"/>
+      </diagonal>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="9"/>
+      </right>
+      <top style="thin">
+        <color theme="9"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF25FF49"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="9"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFF00"/>
+      </right>
+      <top style="thin">
+        <color theme="9"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF25FF49"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border diagonalUp="1" diagonalDown="1">
+      <left/>
+      <right style="medium">
+        <color rgb="FF25FF49"/>
+      </right>
+      <top style="thin">
+        <color theme="9"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF25FF49"/>
+      </bottom>
+      <diagonal style="thin">
+        <color rgb="FFFFFF00"/>
+      </diagonal>
+    </border>
+    <border diagonalUp="1" diagonalDown="1">
+      <left style="thin">
+        <color rgb="FFFFFF00"/>
+      </left>
+      <right style="thin">
+        <color theme="9"/>
+      </right>
+      <top style="thin">
+        <color theme="9"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF25FF49"/>
+      </bottom>
+      <diagonal style="thin">
+        <color rgb="FFFFFF00"/>
+      </diagonal>
+    </border>
+    <border diagonalUp="1" diagonalDown="1">
+      <left style="thin">
+        <color theme="9"/>
+      </left>
+      <right style="thin">
+        <color theme="9"/>
+      </right>
+      <top style="thin">
+        <color theme="9"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF25FF49"/>
+      </bottom>
+      <diagonal style="thin">
+        <color rgb="FFFFFF00"/>
+      </diagonal>
+    </border>
+    <border diagonalUp="1" diagonalDown="1">
+      <left style="thin">
+        <color theme="9"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFF00"/>
+      </right>
+      <top style="thin">
+        <color theme="9"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF25FF49"/>
+      </bottom>
+      <diagonal style="thin">
+        <color rgb="FFFFFF00"/>
+      </diagonal>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFF00"/>
+      </left>
+      <right style="thin">
+        <color theme="9"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF25FF49"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFFFF00"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF25FF49"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF25FF49"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="9"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF25FF49"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -587,12 +1524,340 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="58" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="55" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF25FF49"/>
+      <color rgb="FFEB1DC4"/>
+      <color rgb="FFFFB7F6"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -901,25 +2166,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEFDCF33-E8C0-4CB0-8218-2C2A14609337}">
-  <dimension ref="A1:J90"/>
+  <dimension ref="A1:K90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="G53" sqref="G53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.3984375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.1328125" style="2"/>
-    <col min="4" max="4" width="3.3984375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="3.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="2"/>
+    <col min="4" max="4" width="3.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B1" s="1"/>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="E2" t="s">
         <v>0</v>
       </c>
@@ -927,7 +2193,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="E3" s="22" t="s">
         <v>2</v>
       </c>
@@ -935,40 +2201,48 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="E4" s="22"/>
       <c r="J4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="E5" s="22"/>
       <c r="J5" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="E6" s="22"/>
       <c r="J6" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="E7" s="22"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="E8" s="22"/>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="J8" s="136" t="s">
+        <v>148</v>
+      </c>
+      <c r="K8" s="137"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="E9" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="J9" s="136" t="s">
+        <v>149</v>
+      </c>
+      <c r="K9" s="137"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="4"/>
       <c r="C10" s="5"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="14" t="s">
         <v>40</v>
       </c>
@@ -980,7 +2254,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
         <v>80</v>
       </c>
@@ -991,7 +2265,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="6" t="s">
         <v>41</v>
       </c>
@@ -1000,7 +2274,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
         <v>42</v>
       </c>
@@ -1011,7 +2285,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
         <v>43</v>
       </c>
@@ -1022,7 +2296,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="16" t="s">
         <v>96</v>
       </c>
@@ -1031,7 +2305,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="18" t="s">
         <v>44</v>
       </c>
@@ -1042,7 +2316,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="12" t="s">
         <v>84</v>
       </c>
@@ -1051,7 +2325,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="12" t="s">
         <v>85</v>
       </c>
@@ -1060,7 +2334,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="12" t="s">
         <v>87</v>
       </c>
@@ -1069,7 +2343,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="12" t="s">
         <v>86</v>
       </c>
@@ -1078,7 +2352,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="20" t="s">
         <v>45</v>
       </c>
@@ -1089,7 +2363,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="14" t="s">
         <v>48</v>
       </c>
@@ -1101,7 +2375,7 @@
       </c>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
         <v>47</v>
       </c>
@@ -1113,7 +2387,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="12" t="s">
         <v>50</v>
       </c>
@@ -1124,7 +2398,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="12" t="s">
         <v>49</v>
       </c>
@@ -1136,7 +2410,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="6" t="s">
         <v>51</v>
       </c>
@@ -1147,7 +2421,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="6" t="s">
         <v>52</v>
       </c>
@@ -1159,7 +2433,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="12" t="s">
         <v>53</v>
       </c>
@@ -1170,7 +2444,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="12" t="s">
         <v>54</v>
       </c>
@@ -1182,7 +2456,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="6" t="s">
         <v>55</v>
       </c>
@@ -1193,7 +2467,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32" s="6" t="s">
         <v>56</v>
       </c>
@@ -1205,7 +2479,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" s="12" t="s">
         <v>57</v>
       </c>
@@ -1216,7 +2490,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" s="12" t="s">
         <v>58</v>
       </c>
@@ -1228,7 +2502,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" s="6" t="s">
         <v>59</v>
       </c>
@@ -1239,7 +2513,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" s="6" t="s">
         <v>60</v>
       </c>
@@ -1251,7 +2525,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B37" s="12" t="s">
         <v>61</v>
       </c>
@@ -1262,7 +2536,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" s="12" t="s">
         <v>62</v>
       </c>
@@ -1274,7 +2548,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" s="6" t="s">
         <v>63</v>
       </c>
@@ -1285,7 +2559,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B40" s="6" t="s">
         <v>64</v>
       </c>
@@ -1297,7 +2571,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B41" s="12" t="s">
         <v>65</v>
       </c>
@@ -1308,7 +2582,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B42" s="12" t="s">
         <v>66</v>
       </c>
@@ -1320,7 +2594,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B43" s="6" t="s">
         <v>67</v>
       </c>
@@ -1331,7 +2605,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B44" s="6" t="s">
         <v>68</v>
       </c>
@@ -1343,7 +2617,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B45" s="12" t="s">
         <v>69</v>
       </c>
@@ -1354,7 +2628,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B46" s="12" t="s">
         <v>70</v>
       </c>
@@ -1366,7 +2640,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B47" s="6" t="s">
         <v>71</v>
       </c>
@@ -1377,7 +2651,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B48" s="6" t="s">
         <v>72</v>
       </c>
@@ -1389,7 +2663,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B49" s="12" t="s">
         <v>75</v>
       </c>
@@ -1400,7 +2674,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B50" s="12" t="s">
         <v>76</v>
       </c>
@@ -1412,7 +2686,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B51" s="6" t="s">
         <v>73</v>
       </c>
@@ -1423,7 +2697,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B52" s="6" t="s">
         <v>74</v>
       </c>
@@ -1435,7 +2709,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B53" s="12" t="s">
         <v>88</v>
       </c>
@@ -1446,7 +2720,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B54" s="6" t="s">
         <v>77</v>
       </c>
@@ -1457,7 +2731,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B55" s="6" t="s">
         <v>81</v>
       </c>
@@ -1466,7 +2740,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B56" s="6" t="s">
         <v>78</v>
       </c>
@@ -1477,7 +2751,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B57" s="6" t="s">
         <v>82</v>
       </c>
@@ -1486,7 +2760,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B58" s="6" t="s">
         <v>79</v>
       </c>
@@ -1497,7 +2771,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B59" s="16" t="s">
         <v>83</v>
       </c>
@@ -1506,145 +2780,145 @@
         <v>33</v>
       </c>
     </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B60" s="8"/>
       <c r="C60" s="9"/>
     </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B61" s="8"/>
       <c r="C61" s="9"/>
     </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B62" s="8"/>
       <c r="C62" s="9"/>
     </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B63" s="8"/>
       <c r="C63" s="9"/>
     </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.45">
+    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B64" s="8"/>
       <c r="C64" s="9"/>
     </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B65" s="8"/>
       <c r="C65" s="9"/>
     </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B66" s="8"/>
       <c r="C66" s="9"/>
     </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B67" s="8"/>
       <c r="C67" s="9"/>
     </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B68" s="8"/>
       <c r="C68" s="9"/>
     </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B69" s="8"/>
       <c r="C69" s="9"/>
       <c r="E69" s="22" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B70" s="8"/>
       <c r="C70" s="9"/>
       <c r="E70" s="22"/>
     </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B71" s="8"/>
       <c r="C71" s="9"/>
       <c r="E71" s="22"/>
     </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B72" s="8"/>
       <c r="C72" s="9"/>
       <c r="E72" s="22" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B73" s="8"/>
       <c r="C73" s="9"/>
       <c r="E73" s="22"/>
     </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B74" s="8"/>
       <c r="C74" s="9"/>
       <c r="E74" s="22"/>
     </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B75" s="8"/>
       <c r="C75" s="9"/>
       <c r="E75" s="22"/>
     </row>
-    <row r="76" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="76" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B76" s="8"/>
       <c r="C76" s="9"/>
       <c r="E76" s="22"/>
     </row>
-    <row r="77" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B77" s="8"/>
       <c r="C77" s="9"/>
       <c r="E77" s="22" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="78" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="78" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B78" s="8"/>
       <c r="C78" s="9"/>
       <c r="E78" s="22"/>
     </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="79" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B79" s="8"/>
       <c r="C79" s="9"/>
       <c r="E79" s="22"/>
     </row>
-    <row r="80" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="80" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B80" s="8"/>
       <c r="C80" s="9"/>
       <c r="E80" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B81" s="10"/>
       <c r="C81" s="11"/>
     </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E82" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="83" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E83" s="22" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="84" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E84" s="22"/>
     </row>
-    <row r="85" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E85" s="22"/>
     </row>
-    <row r="86" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E86" s="22"/>
     </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E87" s="22"/>
     </row>
-    <row r="88" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E88" s="22"/>
     </row>
-    <row r="89" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E89" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="90" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B90" s="1"/>
       <c r="C90" s="3"/>
     </row>
@@ -1659,4 +2933,2813 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04098A01-C83B-4743-B006-C8D0145247A0}">
+  <dimension ref="B1:AM83"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="45.7109375" style="89" bestFit="1" customWidth="1"/>
+    <col min="6" max="37" width="2.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E1">
+        <v>0</v>
+      </c>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="25"/>
+      <c r="T1" s="25"/>
+      <c r="U1" s="25"/>
+      <c r="V1" s="25"/>
+      <c r="W1" s="25"/>
+      <c r="X1" s="25"/>
+      <c r="Y1" s="25"/>
+      <c r="Z1" s="25"/>
+      <c r="AA1" s="25"/>
+      <c r="AB1" s="25"/>
+      <c r="AC1" s="25"/>
+      <c r="AD1" s="25"/>
+      <c r="AE1" s="25"/>
+      <c r="AF1" s="25"/>
+      <c r="AG1" s="25"/>
+      <c r="AH1" s="25"/>
+      <c r="AI1" s="25"/>
+      <c r="AJ1" s="25"/>
+      <c r="AK1" s="25"/>
+      <c r="AL1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="2:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="135" t="s">
+        <v>131</v>
+      </c>
+      <c r="E2">
+        <v>32</v>
+      </c>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="25"/>
+      <c r="Q2" s="25"/>
+      <c r="R2" s="25"/>
+      <c r="S2" s="25"/>
+      <c r="T2" s="25"/>
+      <c r="U2" s="25"/>
+      <c r="V2" s="25"/>
+      <c r="W2" s="25"/>
+      <c r="X2" s="25"/>
+      <c r="Y2" s="25"/>
+      <c r="Z2" s="25"/>
+      <c r="AA2" s="25"/>
+      <c r="AB2" s="25"/>
+      <c r="AC2" s="25"/>
+      <c r="AD2" s="25"/>
+      <c r="AE2" s="25"/>
+      <c r="AF2" s="25"/>
+      <c r="AG2" s="25"/>
+      <c r="AH2" s="25"/>
+      <c r="AI2" s="25"/>
+      <c r="AJ2" s="25"/>
+      <c r="AK2" s="25"/>
+      <c r="AL2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="2:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="134" t="s">
+        <v>138</v>
+      </c>
+      <c r="E3">
+        <v>64</v>
+      </c>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="25"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="26"/>
+      <c r="P3" s="26"/>
+      <c r="Q3" s="26"/>
+      <c r="R3" s="26"/>
+      <c r="S3" s="26"/>
+      <c r="T3" s="26"/>
+      <c r="U3" s="25"/>
+      <c r="V3" s="25"/>
+      <c r="W3" s="25"/>
+      <c r="X3" s="25"/>
+      <c r="Y3" s="25"/>
+      <c r="Z3" s="25"/>
+      <c r="AA3" s="25"/>
+      <c r="AB3" s="25"/>
+      <c r="AC3" s="25"/>
+      <c r="AD3" s="25"/>
+      <c r="AE3" s="25"/>
+      <c r="AF3" s="25"/>
+      <c r="AG3" s="25"/>
+      <c r="AH3" s="25"/>
+      <c r="AI3" s="25"/>
+      <c r="AJ3" s="25"/>
+      <c r="AK3" s="25"/>
+      <c r="AL3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="B4" s="132" t="s">
+        <v>137</v>
+      </c>
+      <c r="E4">
+        <v>96</v>
+      </c>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="27"/>
+      <c r="M4" s="51"/>
+      <c r="N4" s="52"/>
+      <c r="O4" s="52"/>
+      <c r="P4" s="65"/>
+      <c r="Q4" s="52"/>
+      <c r="R4" s="52"/>
+      <c r="S4" s="52"/>
+      <c r="T4" s="53"/>
+      <c r="U4" s="28"/>
+      <c r="V4" s="25"/>
+      <c r="W4" s="25"/>
+      <c r="X4" s="25"/>
+      <c r="Y4" s="25"/>
+      <c r="Z4" s="25"/>
+      <c r="AA4" s="25"/>
+      <c r="AB4" s="25"/>
+      <c r="AC4" s="25"/>
+      <c r="AD4" s="25"/>
+      <c r="AE4" s="25"/>
+      <c r="AF4" s="25"/>
+      <c r="AG4" s="25"/>
+      <c r="AH4" s="25"/>
+      <c r="AI4" s="25"/>
+      <c r="AJ4" s="25"/>
+      <c r="AK4" s="25"/>
+      <c r="AL4">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="B5" s="132"/>
+      <c r="E5">
+        <v>128</v>
+      </c>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="27"/>
+      <c r="M5" s="54"/>
+      <c r="N5" s="29"/>
+      <c r="O5" s="63"/>
+      <c r="P5" s="62"/>
+      <c r="Q5" s="39"/>
+      <c r="R5" s="29"/>
+      <c r="S5" s="29"/>
+      <c r="T5" s="55"/>
+      <c r="U5" s="28"/>
+      <c r="V5" s="25"/>
+      <c r="W5" s="25"/>
+      <c r="X5" s="25"/>
+      <c r="Y5" s="25"/>
+      <c r="Z5" s="25"/>
+      <c r="AA5" s="25"/>
+      <c r="AB5" s="25"/>
+      <c r="AC5" s="25"/>
+      <c r="AD5" s="25"/>
+      <c r="AE5" s="25"/>
+      <c r="AF5" s="25"/>
+      <c r="AG5" s="25"/>
+      <c r="AH5" s="25"/>
+      <c r="AI5" s="25"/>
+      <c r="AJ5" s="25"/>
+      <c r="AK5" s="25"/>
+      <c r="AL5">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="6" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="B6" s="132" t="s">
+        <v>135</v>
+      </c>
+      <c r="E6">
+        <v>160</v>
+      </c>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="27"/>
+      <c r="M6" s="54"/>
+      <c r="N6" s="29"/>
+      <c r="O6" s="29"/>
+      <c r="P6" s="66"/>
+      <c r="Q6" s="33"/>
+      <c r="R6" s="29"/>
+      <c r="S6" s="29"/>
+      <c r="T6" s="55"/>
+      <c r="U6" s="28"/>
+      <c r="V6" s="25"/>
+      <c r="W6" s="25"/>
+      <c r="X6" s="25"/>
+      <c r="Y6" s="25"/>
+      <c r="Z6" s="25"/>
+      <c r="AA6" s="25"/>
+      <c r="AB6" s="25"/>
+      <c r="AC6" s="25"/>
+      <c r="AD6" s="25"/>
+      <c r="AE6" s="25"/>
+      <c r="AF6" s="25"/>
+      <c r="AG6" s="25"/>
+      <c r="AH6" s="25"/>
+      <c r="AI6" s="25"/>
+      <c r="AJ6" s="25"/>
+      <c r="AK6" s="25"/>
+      <c r="AL6">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="7" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="B7" s="132" t="s">
+        <v>139</v>
+      </c>
+      <c r="E7">
+        <v>192</v>
+      </c>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="25"/>
+      <c r="L7" s="27"/>
+      <c r="M7" s="54"/>
+      <c r="N7" s="29"/>
+      <c r="O7" s="29"/>
+      <c r="P7" s="33"/>
+      <c r="Q7" s="33"/>
+      <c r="R7" s="29"/>
+      <c r="S7" s="29"/>
+      <c r="T7" s="55"/>
+      <c r="U7" s="28"/>
+      <c r="V7" s="25"/>
+      <c r="W7" s="25"/>
+      <c r="X7" s="25"/>
+      <c r="Y7" s="25"/>
+      <c r="Z7" s="25"/>
+      <c r="AA7" s="25"/>
+      <c r="AB7" s="25"/>
+      <c r="AC7" s="25"/>
+      <c r="AD7" s="25"/>
+      <c r="AE7" s="25"/>
+      <c r="AF7" s="25"/>
+      <c r="AG7" s="25"/>
+      <c r="AH7" s="25"/>
+      <c r="AI7" s="25"/>
+      <c r="AJ7" s="25"/>
+      <c r="AK7" s="25"/>
+      <c r="AL7">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="8" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="B8" s="132" t="s">
+        <v>140</v>
+      </c>
+      <c r="E8">
+        <v>224</v>
+      </c>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="25"/>
+      <c r="L8" s="27"/>
+      <c r="M8" s="54"/>
+      <c r="N8" s="29"/>
+      <c r="O8" s="29"/>
+      <c r="P8" s="30"/>
+      <c r="Q8" s="33"/>
+      <c r="R8" s="29"/>
+      <c r="S8" s="29"/>
+      <c r="T8" s="55"/>
+      <c r="U8" s="28"/>
+      <c r="V8" s="25"/>
+      <c r="W8" s="25"/>
+      <c r="X8" s="25"/>
+      <c r="Y8" s="25"/>
+      <c r="Z8" s="25"/>
+      <c r="AA8" s="25"/>
+      <c r="AB8" s="25"/>
+      <c r="AC8" s="25"/>
+      <c r="AD8" s="25"/>
+      <c r="AE8" s="25"/>
+      <c r="AF8" s="25"/>
+      <c r="AG8" s="25"/>
+      <c r="AH8" s="25"/>
+      <c r="AI8" s="25"/>
+      <c r="AJ8" s="25"/>
+      <c r="AK8" s="25"/>
+      <c r="AL8">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="9" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="B9" s="132"/>
+      <c r="E9">
+        <v>256</v>
+      </c>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="27"/>
+      <c r="M9" s="54"/>
+      <c r="N9" s="29"/>
+      <c r="O9" s="29"/>
+      <c r="P9" s="33"/>
+      <c r="Q9" s="64"/>
+      <c r="R9" s="29"/>
+      <c r="S9" s="29"/>
+      <c r="T9" s="55"/>
+      <c r="U9" s="28"/>
+      <c r="V9" s="25"/>
+      <c r="W9" s="25"/>
+      <c r="X9" s="25"/>
+      <c r="Y9" s="25"/>
+      <c r="Z9" s="25"/>
+      <c r="AA9" s="25"/>
+      <c r="AB9" s="25"/>
+      <c r="AC9" s="25"/>
+      <c r="AD9" s="25"/>
+      <c r="AE9" s="25"/>
+      <c r="AF9" s="25"/>
+      <c r="AG9" s="25"/>
+      <c r="AH9" s="25"/>
+      <c r="AI9" s="25"/>
+      <c r="AJ9" s="25"/>
+      <c r="AK9" s="25"/>
+      <c r="AL9">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="10" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="B10" s="132" t="s">
+        <v>136</v>
+      </c>
+      <c r="E10">
+        <v>288</v>
+      </c>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="27"/>
+      <c r="M10" s="54"/>
+      <c r="N10" s="29"/>
+      <c r="O10" s="29"/>
+      <c r="P10" s="63"/>
+      <c r="Q10" s="62"/>
+      <c r="R10" s="39"/>
+      <c r="S10" s="29"/>
+      <c r="T10" s="55"/>
+      <c r="U10" s="28"/>
+      <c r="V10" s="25"/>
+      <c r="W10" s="25"/>
+      <c r="X10" s="25"/>
+      <c r="Y10" s="25"/>
+      <c r="Z10" s="25"/>
+      <c r="AA10" s="25"/>
+      <c r="AB10" s="25"/>
+      <c r="AC10" s="25"/>
+      <c r="AD10" s="25"/>
+      <c r="AE10" s="25"/>
+      <c r="AF10" s="25"/>
+      <c r="AG10" s="25"/>
+      <c r="AH10" s="25"/>
+      <c r="AI10" s="25"/>
+      <c r="AJ10" s="25"/>
+      <c r="AK10" s="25"/>
+      <c r="AL10">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="11" spans="2:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="132" t="s">
+        <v>141</v>
+      </c>
+      <c r="E11">
+        <v>320</v>
+      </c>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="27"/>
+      <c r="M11" s="56"/>
+      <c r="N11" s="57"/>
+      <c r="O11" s="57"/>
+      <c r="P11" s="57"/>
+      <c r="Q11" s="59"/>
+      <c r="R11" s="57"/>
+      <c r="S11" s="57"/>
+      <c r="T11" s="58"/>
+      <c r="U11" s="28"/>
+      <c r="V11" s="25"/>
+      <c r="W11" s="25"/>
+      <c r="X11" s="25"/>
+      <c r="Y11" s="25"/>
+      <c r="Z11" s="25"/>
+      <c r="AA11" s="25"/>
+      <c r="AB11" s="25"/>
+      <c r="AC11" s="25"/>
+      <c r="AD11" s="25"/>
+      <c r="AE11" s="25"/>
+      <c r="AF11" s="25"/>
+      <c r="AG11" s="25"/>
+      <c r="AH11" s="25"/>
+      <c r="AI11" s="25"/>
+      <c r="AJ11" s="25"/>
+      <c r="AK11" s="25"/>
+      <c r="AL11">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="12" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="B12" s="132" t="s">
+        <v>142</v>
+      </c>
+      <c r="E12">
+        <v>352</v>
+      </c>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="25"/>
+      <c r="L12" s="25"/>
+      <c r="M12" s="35"/>
+      <c r="N12" s="35"/>
+      <c r="O12" s="35"/>
+      <c r="P12" s="35"/>
+      <c r="Q12" s="35"/>
+      <c r="R12" s="35"/>
+      <c r="S12" s="35"/>
+      <c r="T12" s="35"/>
+      <c r="U12" s="25"/>
+      <c r="V12" s="25"/>
+      <c r="W12" s="25"/>
+      <c r="X12" s="25"/>
+      <c r="Y12" s="25"/>
+      <c r="Z12" s="25"/>
+      <c r="AA12" s="25"/>
+      <c r="AB12" s="25"/>
+      <c r="AC12" s="25"/>
+      <c r="AD12" s="25"/>
+      <c r="AE12" s="25"/>
+      <c r="AF12" s="25"/>
+      <c r="AG12" s="25"/>
+      <c r="AH12" s="25"/>
+      <c r="AI12" s="25"/>
+      <c r="AJ12" s="25"/>
+      <c r="AK12" s="25"/>
+      <c r="AL12">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="13" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="B13" s="132"/>
+      <c r="E13">
+        <v>384</v>
+      </c>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="25"/>
+      <c r="K13" s="25"/>
+      <c r="L13" s="25"/>
+      <c r="M13" s="25"/>
+      <c r="N13" s="25"/>
+      <c r="O13" s="25"/>
+      <c r="P13" s="25"/>
+      <c r="Q13" s="25"/>
+      <c r="R13" s="25"/>
+      <c r="S13" s="25"/>
+      <c r="T13" s="25"/>
+      <c r="U13" s="25"/>
+      <c r="V13" s="25"/>
+      <c r="W13" s="25"/>
+      <c r="X13" s="25"/>
+      <c r="Y13" s="25"/>
+      <c r="Z13" s="25"/>
+      <c r="AA13" s="25"/>
+      <c r="AB13" s="25"/>
+      <c r="AC13" s="25"/>
+      <c r="AD13" s="25"/>
+      <c r="AE13" s="25"/>
+      <c r="AF13" s="25"/>
+      <c r="AG13" s="25"/>
+      <c r="AH13" s="25"/>
+      <c r="AI13" s="25"/>
+      <c r="AJ13" s="25"/>
+      <c r="AK13" s="25"/>
+      <c r="AL13">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="14" spans="2:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="132" t="s">
+        <v>143</v>
+      </c>
+      <c r="E14">
+        <v>416</v>
+      </c>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="26"/>
+      <c r="L14" s="26"/>
+      <c r="M14" s="26"/>
+      <c r="N14" s="26"/>
+      <c r="O14" s="26"/>
+      <c r="P14" s="26"/>
+      <c r="Q14" s="26"/>
+      <c r="R14" s="26"/>
+      <c r="S14" s="26"/>
+      <c r="T14" s="26"/>
+      <c r="U14" s="26"/>
+      <c r="V14" s="26"/>
+      <c r="W14" s="26"/>
+      <c r="X14" s="26"/>
+      <c r="Y14" s="26"/>
+      <c r="Z14" s="26"/>
+      <c r="AA14" s="25"/>
+      <c r="AB14" s="25"/>
+      <c r="AC14" s="25"/>
+      <c r="AD14" s="25"/>
+      <c r="AE14" s="25"/>
+      <c r="AF14" s="25"/>
+      <c r="AG14" s="25"/>
+      <c r="AH14" s="25"/>
+      <c r="AI14" s="25"/>
+      <c r="AJ14" s="25"/>
+      <c r="AK14" s="25"/>
+      <c r="AL14">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="15" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="B15" s="132" t="s">
+        <v>144</v>
+      </c>
+      <c r="E15">
+        <v>448</v>
+      </c>
+      <c r="F15" s="25">
+        <v>448</v>
+      </c>
+      <c r="G15" s="25">
+        <v>449</v>
+      </c>
+      <c r="H15" s="25">
+        <v>450</v>
+      </c>
+      <c r="I15" s="25">
+        <v>451</v>
+      </c>
+      <c r="J15" s="27">
+        <v>452</v>
+      </c>
+      <c r="K15" s="80">
+        <v>453</v>
+      </c>
+      <c r="L15" s="60"/>
+      <c r="M15" s="60"/>
+      <c r="N15" s="60"/>
+      <c r="O15" s="60"/>
+      <c r="P15" s="60"/>
+      <c r="Q15" s="60"/>
+      <c r="R15" s="61"/>
+      <c r="S15" s="61"/>
+      <c r="T15" s="60"/>
+      <c r="U15" s="60"/>
+      <c r="V15" s="60"/>
+      <c r="W15" s="60"/>
+      <c r="X15" s="60"/>
+      <c r="Y15" s="60"/>
+      <c r="Z15" s="67">
+        <v>468</v>
+      </c>
+      <c r="AA15" s="28">
+        <v>469</v>
+      </c>
+      <c r="AB15" s="25">
+        <v>470</v>
+      </c>
+      <c r="AC15" s="25">
+        <v>471</v>
+      </c>
+      <c r="AD15" s="25">
+        <v>472</v>
+      </c>
+      <c r="AE15" s="25">
+        <v>473</v>
+      </c>
+      <c r="AF15" s="25">
+        <v>474</v>
+      </c>
+      <c r="AG15" s="25">
+        <v>475</v>
+      </c>
+      <c r="AH15" s="25">
+        <v>476</v>
+      </c>
+      <c r="AI15" s="25">
+        <v>477</v>
+      </c>
+      <c r="AJ15" s="25">
+        <v>478</v>
+      </c>
+      <c r="AK15" s="25">
+        <v>479</v>
+      </c>
+      <c r="AL15">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="16" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="B16" s="132" t="s">
+        <v>145</v>
+      </c>
+      <c r="E16">
+        <v>480</v>
+      </c>
+      <c r="F16" s="25">
+        <v>480</v>
+      </c>
+      <c r="G16" s="25">
+        <v>481</v>
+      </c>
+      <c r="H16" s="25">
+        <v>482</v>
+      </c>
+      <c r="I16" s="25">
+        <v>483</v>
+      </c>
+      <c r="J16" s="27">
+        <v>484</v>
+      </c>
+      <c r="K16" s="90">
+        <v>485</v>
+      </c>
+      <c r="L16" s="38"/>
+      <c r="M16" s="36"/>
+      <c r="N16" s="82"/>
+      <c r="O16" s="36"/>
+      <c r="P16" s="36"/>
+      <c r="Q16" s="36"/>
+      <c r="R16" s="37"/>
+      <c r="S16" s="37"/>
+      <c r="T16" s="36"/>
+      <c r="U16" s="36"/>
+      <c r="V16" s="36"/>
+      <c r="W16" s="36"/>
+      <c r="X16" s="36"/>
+      <c r="Y16" s="42"/>
+      <c r="Z16" s="78">
+        <v>500</v>
+      </c>
+      <c r="AA16" s="28">
+        <v>501</v>
+      </c>
+      <c r="AB16" s="25">
+        <v>502</v>
+      </c>
+      <c r="AC16" s="25">
+        <v>503</v>
+      </c>
+      <c r="AD16" s="25">
+        <v>504</v>
+      </c>
+      <c r="AE16" s="25">
+        <v>505</v>
+      </c>
+      <c r="AF16" s="25">
+        <v>506</v>
+      </c>
+      <c r="AG16" s="25">
+        <v>507</v>
+      </c>
+      <c r="AH16" s="25">
+        <v>508</v>
+      </c>
+      <c r="AI16" s="25">
+        <v>509</v>
+      </c>
+      <c r="AJ16" s="25">
+        <v>510</v>
+      </c>
+      <c r="AK16" s="25">
+        <v>511</v>
+      </c>
+      <c r="AL16">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="17" spans="2:39" x14ac:dyDescent="0.25">
+      <c r="B17" s="132" t="s">
+        <v>146</v>
+      </c>
+      <c r="E17">
+        <v>512</v>
+      </c>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="75"/>
+      <c r="L17" s="39"/>
+      <c r="M17" s="43"/>
+      <c r="N17" s="29"/>
+      <c r="O17" s="39"/>
+      <c r="P17" s="29"/>
+      <c r="Q17" s="29"/>
+      <c r="R17" s="31"/>
+      <c r="S17" s="31"/>
+      <c r="T17" s="29"/>
+      <c r="U17" s="29"/>
+      <c r="V17" s="29"/>
+      <c r="W17" s="29"/>
+      <c r="X17" s="29"/>
+      <c r="Y17" s="43"/>
+      <c r="Z17" s="78">
+        <v>532</v>
+      </c>
+      <c r="AA17" s="28"/>
+      <c r="AB17" s="25"/>
+      <c r="AC17" s="25"/>
+      <c r="AD17" s="25"/>
+      <c r="AE17" s="25"/>
+      <c r="AF17" s="25"/>
+      <c r="AG17" s="25"/>
+      <c r="AH17" s="25"/>
+      <c r="AI17" s="25"/>
+      <c r="AJ17" s="25"/>
+      <c r="AK17" s="25"/>
+      <c r="AL17">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="18" spans="2:39" x14ac:dyDescent="0.25">
+      <c r="B18" s="132" t="s">
+        <v>159</v>
+      </c>
+      <c r="E18">
+        <v>544</v>
+      </c>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="25"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="75"/>
+      <c r="L18" s="39"/>
+      <c r="M18" s="29"/>
+      <c r="N18" s="36"/>
+      <c r="O18" s="29"/>
+      <c r="P18" s="29"/>
+      <c r="Q18" s="29"/>
+      <c r="R18" s="32"/>
+      <c r="S18" s="32"/>
+      <c r="T18" s="29"/>
+      <c r="U18" s="29"/>
+      <c r="V18" s="29"/>
+      <c r="W18" s="29"/>
+      <c r="X18" s="29"/>
+      <c r="Y18" s="43"/>
+      <c r="Z18" s="78">
+        <v>564</v>
+      </c>
+      <c r="AA18" s="28"/>
+      <c r="AB18" s="25"/>
+      <c r="AC18" s="25"/>
+      <c r="AD18" s="25"/>
+      <c r="AE18" s="25"/>
+      <c r="AF18" s="25"/>
+      <c r="AG18" s="25"/>
+      <c r="AH18" s="25"/>
+      <c r="AI18" s="25"/>
+      <c r="AJ18" s="25"/>
+      <c r="AK18" s="25"/>
+      <c r="AL18">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="19" spans="2:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="133" t="s">
+        <v>147</v>
+      </c>
+      <c r="E19">
+        <v>576</v>
+      </c>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="25"/>
+      <c r="I19" s="25"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="75"/>
+      <c r="L19" s="39"/>
+      <c r="M19" s="29"/>
+      <c r="N19" s="29"/>
+      <c r="O19" s="29"/>
+      <c r="P19" s="29"/>
+      <c r="Q19" s="31"/>
+      <c r="R19" s="32"/>
+      <c r="S19" s="32"/>
+      <c r="T19" s="31"/>
+      <c r="U19" s="29"/>
+      <c r="V19" s="29"/>
+      <c r="W19" s="29"/>
+      <c r="X19" s="29"/>
+      <c r="Y19" s="43"/>
+      <c r="Z19" s="78">
+        <v>596</v>
+      </c>
+      <c r="AA19" s="28"/>
+      <c r="AB19" s="25"/>
+      <c r="AC19" s="25"/>
+      <c r="AD19" s="25"/>
+      <c r="AE19" s="25"/>
+      <c r="AF19" s="25"/>
+      <c r="AG19" s="25"/>
+      <c r="AH19" s="25"/>
+      <c r="AI19" s="25"/>
+      <c r="AJ19" s="25"/>
+      <c r="AK19" s="25"/>
+      <c r="AL19">
+        <v>607</v>
+      </c>
+      <c r="AM19" s="76"/>
+    </row>
+    <row r="20" spans="2:39" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <v>608</v>
+      </c>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="25"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="75"/>
+      <c r="L20" s="39"/>
+      <c r="M20" s="29"/>
+      <c r="N20" s="33"/>
+      <c r="O20" s="29"/>
+      <c r="P20" s="29"/>
+      <c r="Q20" s="31"/>
+      <c r="R20" s="32"/>
+      <c r="S20" s="32"/>
+      <c r="T20" s="31"/>
+      <c r="U20" s="29"/>
+      <c r="V20" s="29"/>
+      <c r="W20" s="33"/>
+      <c r="X20" s="29"/>
+      <c r="Y20" s="43"/>
+      <c r="Z20" s="78">
+        <v>628</v>
+      </c>
+      <c r="AA20" s="28"/>
+      <c r="AB20" s="25"/>
+      <c r="AC20" s="25"/>
+      <c r="AD20" s="25"/>
+      <c r="AE20" s="25"/>
+      <c r="AF20" s="25"/>
+      <c r="AG20" s="25"/>
+      <c r="AH20" s="25"/>
+      <c r="AI20" s="25"/>
+      <c r="AJ20" s="25"/>
+      <c r="AK20" s="25"/>
+      <c r="AL20">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="21" spans="2:39" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <v>640</v>
+      </c>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="25"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="75"/>
+      <c r="L21" s="39"/>
+      <c r="M21" s="29"/>
+      <c r="N21" s="30"/>
+      <c r="O21" s="29"/>
+      <c r="P21" s="29"/>
+      <c r="Q21" s="32"/>
+      <c r="R21" s="32"/>
+      <c r="S21" s="32"/>
+      <c r="T21" s="32"/>
+      <c r="U21" s="29"/>
+      <c r="V21" s="29"/>
+      <c r="W21" s="30"/>
+      <c r="X21" s="29"/>
+      <c r="Y21" s="43"/>
+      <c r="Z21" s="78">
+        <v>660</v>
+      </c>
+      <c r="AA21" s="28"/>
+      <c r="AB21" s="25"/>
+      <c r="AC21" s="25"/>
+      <c r="AD21" s="25"/>
+      <c r="AE21" s="25"/>
+      <c r="AF21" s="25"/>
+      <c r="AG21" s="25"/>
+      <c r="AH21" s="25"/>
+      <c r="AI21" s="25"/>
+      <c r="AJ21" s="25"/>
+      <c r="AK21" s="25"/>
+      <c r="AL21">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="22" spans="2:39" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <v>672</v>
+      </c>
+      <c r="F22" s="25"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="25"/>
+      <c r="I22" s="25"/>
+      <c r="J22" s="27"/>
+      <c r="K22" s="75"/>
+      <c r="L22" s="39"/>
+      <c r="M22" s="29"/>
+      <c r="N22" s="31"/>
+      <c r="O22" s="29"/>
+      <c r="P22" s="31"/>
+      <c r="Q22" s="32"/>
+      <c r="R22" s="32"/>
+      <c r="S22" s="32"/>
+      <c r="T22" s="32"/>
+      <c r="U22" s="31"/>
+      <c r="V22" s="29"/>
+      <c r="W22" s="31"/>
+      <c r="X22" s="29"/>
+      <c r="Y22" s="43"/>
+      <c r="Z22" s="78">
+        <v>692</v>
+      </c>
+      <c r="AA22" s="28"/>
+      <c r="AB22" s="25"/>
+      <c r="AC22" s="25"/>
+      <c r="AD22" s="25"/>
+      <c r="AE22" s="25"/>
+      <c r="AF22" s="25"/>
+      <c r="AG22" s="25"/>
+      <c r="AH22" s="25"/>
+      <c r="AI22" s="25"/>
+      <c r="AJ22" s="25"/>
+      <c r="AK22" s="25"/>
+      <c r="AL22">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="23" spans="2:39" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <v>704</v>
+      </c>
+      <c r="F23" s="25"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="25"/>
+      <c r="I23" s="25"/>
+      <c r="J23" s="27"/>
+      <c r="K23" s="68"/>
+      <c r="L23" s="39"/>
+      <c r="M23" s="29"/>
+      <c r="N23" s="32"/>
+      <c r="O23" s="34"/>
+      <c r="P23" s="32"/>
+      <c r="Q23" s="32"/>
+      <c r="R23" s="33"/>
+      <c r="S23" s="33"/>
+      <c r="T23" s="32"/>
+      <c r="U23" s="32"/>
+      <c r="V23" s="34"/>
+      <c r="W23" s="32"/>
+      <c r="X23" s="29"/>
+      <c r="Y23" s="43"/>
+      <c r="Z23" s="70"/>
+      <c r="AA23" s="28"/>
+      <c r="AB23" s="25"/>
+      <c r="AC23" s="25"/>
+      <c r="AD23" s="25"/>
+      <c r="AE23" s="25"/>
+      <c r="AF23" s="25"/>
+      <c r="AG23" s="25"/>
+      <c r="AH23" s="25"/>
+      <c r="AI23" s="25"/>
+      <c r="AJ23" s="25"/>
+      <c r="AK23" s="25"/>
+      <c r="AL23">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="24" spans="2:39" x14ac:dyDescent="0.25">
+      <c r="E24">
+        <v>736</v>
+      </c>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="25"/>
+      <c r="I24" s="25"/>
+      <c r="J24" s="27"/>
+      <c r="K24" s="69"/>
+      <c r="L24" s="39"/>
+      <c r="M24" s="29"/>
+      <c r="N24" s="34"/>
+      <c r="O24" s="32"/>
+      <c r="P24" s="32"/>
+      <c r="Q24" s="33"/>
+      <c r="R24" s="33"/>
+      <c r="S24" s="33"/>
+      <c r="T24" s="33"/>
+      <c r="U24" s="32"/>
+      <c r="V24" s="32"/>
+      <c r="W24" s="34"/>
+      <c r="X24" s="29"/>
+      <c r="Y24" s="43"/>
+      <c r="Z24" s="71"/>
+      <c r="AA24" s="28"/>
+      <c r="AB24" s="25"/>
+      <c r="AC24" s="25"/>
+      <c r="AD24" s="25"/>
+      <c r="AE24" s="25"/>
+      <c r="AF24" s="25"/>
+      <c r="AG24" s="25"/>
+      <c r="AH24" s="25"/>
+      <c r="AI24" s="25"/>
+      <c r="AJ24" s="25"/>
+      <c r="AK24" s="25"/>
+      <c r="AL24">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="25" spans="2:39" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <v>768</v>
+      </c>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="25"/>
+      <c r="I25" s="25"/>
+      <c r="J25" s="27"/>
+      <c r="K25" s="74"/>
+      <c r="L25" s="39"/>
+      <c r="M25" s="29"/>
+      <c r="N25" s="32"/>
+      <c r="O25" s="32"/>
+      <c r="P25" s="32"/>
+      <c r="Q25" s="33"/>
+      <c r="R25" s="32"/>
+      <c r="S25" s="32"/>
+      <c r="T25" s="33"/>
+      <c r="U25" s="32"/>
+      <c r="V25" s="32"/>
+      <c r="W25" s="32"/>
+      <c r="X25" s="29"/>
+      <c r="Y25" s="43"/>
+      <c r="Z25" s="72"/>
+      <c r="AA25" s="28"/>
+      <c r="AB25" s="25"/>
+      <c r="AC25" s="25"/>
+      <c r="AD25" s="25"/>
+      <c r="AE25" s="25"/>
+      <c r="AF25" s="25"/>
+      <c r="AG25" s="25"/>
+      <c r="AH25" s="25"/>
+      <c r="AI25" s="25"/>
+      <c r="AJ25" s="25"/>
+      <c r="AK25" s="25"/>
+      <c r="AL25">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="26" spans="2:39" x14ac:dyDescent="0.25">
+      <c r="E26">
+        <v>800</v>
+      </c>
+      <c r="F26" s="25"/>
+      <c r="G26" s="25"/>
+      <c r="H26" s="25"/>
+      <c r="I26" s="25"/>
+      <c r="J26" s="27"/>
+      <c r="K26" s="73"/>
+      <c r="L26" s="39"/>
+      <c r="M26" s="31"/>
+      <c r="N26" s="32"/>
+      <c r="O26" s="32"/>
+      <c r="P26" s="31"/>
+      <c r="Q26" s="32"/>
+      <c r="R26" s="32"/>
+      <c r="S26" s="32"/>
+      <c r="T26" s="32"/>
+      <c r="U26" s="31"/>
+      <c r="V26" s="32"/>
+      <c r="W26" s="32"/>
+      <c r="X26" s="31"/>
+      <c r="Y26" s="43"/>
+      <c r="Z26" s="77"/>
+      <c r="AA26" s="28"/>
+      <c r="AB26" s="25"/>
+      <c r="AC26" s="25"/>
+      <c r="AD26" s="25"/>
+      <c r="AE26" s="25"/>
+      <c r="AF26" s="25"/>
+      <c r="AG26" s="25"/>
+      <c r="AH26" s="25"/>
+      <c r="AI26" s="25"/>
+      <c r="AJ26" s="25"/>
+      <c r="AK26" s="25"/>
+      <c r="AL26">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="27" spans="2:39" x14ac:dyDescent="0.25">
+      <c r="E27">
+        <v>832</v>
+      </c>
+      <c r="F27" s="25"/>
+      <c r="G27" s="25"/>
+      <c r="H27" s="25"/>
+      <c r="I27" s="25"/>
+      <c r="J27" s="27"/>
+      <c r="K27" s="73"/>
+      <c r="L27" s="40"/>
+      <c r="M27" s="32"/>
+      <c r="N27" s="32"/>
+      <c r="O27" s="31"/>
+      <c r="P27" s="30"/>
+      <c r="Q27" s="31"/>
+      <c r="R27" s="32"/>
+      <c r="S27" s="32"/>
+      <c r="T27" s="31"/>
+      <c r="U27" s="30"/>
+      <c r="V27" s="31"/>
+      <c r="W27" s="32"/>
+      <c r="X27" s="32"/>
+      <c r="Y27" s="44"/>
+      <c r="Z27" s="77"/>
+      <c r="AA27" s="28"/>
+      <c r="AB27" s="25"/>
+      <c r="AC27" s="25"/>
+      <c r="AD27" s="25"/>
+      <c r="AE27" s="25"/>
+      <c r="AF27" s="25"/>
+      <c r="AG27" s="25"/>
+      <c r="AH27" s="25"/>
+      <c r="AI27" s="25"/>
+      <c r="AJ27" s="25"/>
+      <c r="AK27" s="25"/>
+      <c r="AL27">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="28" spans="2:39" x14ac:dyDescent="0.25">
+      <c r="E28">
+        <v>864</v>
+      </c>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="27"/>
+      <c r="K28" s="73"/>
+      <c r="L28" s="41"/>
+      <c r="M28" s="32"/>
+      <c r="N28" s="29"/>
+      <c r="O28" s="33"/>
+      <c r="P28" s="30"/>
+      <c r="Q28" s="31"/>
+      <c r="R28" s="32"/>
+      <c r="S28" s="32"/>
+      <c r="T28" s="31"/>
+      <c r="U28" s="30"/>
+      <c r="V28" s="33"/>
+      <c r="W28" s="29"/>
+      <c r="X28" s="32"/>
+      <c r="Y28" s="45"/>
+      <c r="Z28" s="77"/>
+      <c r="AA28" s="28"/>
+      <c r="AB28" s="25"/>
+      <c r="AC28" s="25"/>
+      <c r="AD28" s="25"/>
+      <c r="AE28" s="25"/>
+      <c r="AF28" s="25"/>
+      <c r="AG28" s="25"/>
+      <c r="AH28" s="25"/>
+      <c r="AI28" s="25"/>
+      <c r="AJ28" s="25"/>
+      <c r="AK28" s="25"/>
+      <c r="AL28">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="29" spans="2:39" x14ac:dyDescent="0.25">
+      <c r="E29">
+        <v>896</v>
+      </c>
+      <c r="F29" s="25"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="25"/>
+      <c r="I29" s="25"/>
+      <c r="J29" s="27"/>
+      <c r="K29" s="81"/>
+      <c r="L29" s="46"/>
+      <c r="M29" s="47"/>
+      <c r="N29" s="47"/>
+      <c r="O29" s="48"/>
+      <c r="P29" s="48"/>
+      <c r="Q29" s="47"/>
+      <c r="R29" s="49"/>
+      <c r="S29" s="49"/>
+      <c r="T29" s="47"/>
+      <c r="U29" s="48"/>
+      <c r="V29" s="48"/>
+      <c r="W29" s="47"/>
+      <c r="X29" s="47"/>
+      <c r="Y29" s="50"/>
+      <c r="Z29" s="83"/>
+      <c r="AA29" s="28"/>
+      <c r="AB29" s="25"/>
+      <c r="AC29" s="25"/>
+      <c r="AD29" s="25"/>
+      <c r="AE29" s="25"/>
+      <c r="AF29" s="25"/>
+      <c r="AG29" s="25"/>
+      <c r="AH29" s="25"/>
+      <c r="AI29" s="25"/>
+      <c r="AJ29" s="25"/>
+      <c r="AK29" s="25"/>
+      <c r="AL29">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="30" spans="2:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E30">
+        <v>928</v>
+      </c>
+      <c r="F30" s="25"/>
+      <c r="G30" s="25"/>
+      <c r="H30" s="25"/>
+      <c r="I30" s="25"/>
+      <c r="J30" s="27"/>
+      <c r="K30" s="86"/>
+      <c r="L30" s="85"/>
+      <c r="M30" s="57"/>
+      <c r="N30" s="57"/>
+      <c r="O30" s="57"/>
+      <c r="P30" s="57"/>
+      <c r="Q30" s="57"/>
+      <c r="R30" s="84"/>
+      <c r="S30" s="84"/>
+      <c r="T30" s="57"/>
+      <c r="U30" s="57"/>
+      <c r="V30" s="57"/>
+      <c r="W30" s="57"/>
+      <c r="X30" s="57"/>
+      <c r="Y30" s="88"/>
+      <c r="Z30" s="87">
+        <v>948</v>
+      </c>
+      <c r="AA30" s="28">
+        <v>949</v>
+      </c>
+      <c r="AB30" s="25">
+        <v>950</v>
+      </c>
+      <c r="AC30" s="25">
+        <v>951</v>
+      </c>
+      <c r="AD30" s="25">
+        <v>952</v>
+      </c>
+      <c r="AE30" s="25">
+        <v>953</v>
+      </c>
+      <c r="AF30" s="25">
+        <v>954</v>
+      </c>
+      <c r="AG30" s="25">
+        <v>955</v>
+      </c>
+      <c r="AH30" s="25">
+        <v>956</v>
+      </c>
+      <c r="AI30" s="25">
+        <v>957</v>
+      </c>
+      <c r="AJ30" s="25">
+        <v>958</v>
+      </c>
+      <c r="AK30" s="25">
+        <v>959</v>
+      </c>
+      <c r="AL30">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="31" spans="2:39" x14ac:dyDescent="0.25">
+      <c r="E31">
+        <v>960</v>
+      </c>
+      <c r="F31" s="25"/>
+      <c r="G31" s="25"/>
+      <c r="H31" s="25"/>
+      <c r="I31" s="25"/>
+      <c r="J31" s="25"/>
+      <c r="K31" s="35"/>
+      <c r="L31" s="35"/>
+      <c r="M31" s="35"/>
+      <c r="N31" s="35"/>
+      <c r="O31" s="35"/>
+      <c r="P31" s="35"/>
+      <c r="Q31" s="35"/>
+      <c r="R31" s="35"/>
+      <c r="S31" s="35"/>
+      <c r="T31" s="35"/>
+      <c r="U31" s="35"/>
+      <c r="V31" s="35"/>
+      <c r="W31" s="35"/>
+      <c r="X31" s="35"/>
+      <c r="Y31" s="35"/>
+      <c r="Z31" s="35"/>
+      <c r="AA31" s="25"/>
+      <c r="AB31" s="25"/>
+      <c r="AC31" s="25"/>
+      <c r="AD31" s="25"/>
+      <c r="AE31" s="25"/>
+      <c r="AF31" s="25"/>
+      <c r="AG31" s="25"/>
+      <c r="AH31" s="25"/>
+      <c r="AI31" s="25"/>
+      <c r="AJ31" s="25"/>
+      <c r="AK31" s="25"/>
+      <c r="AL31">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="32" spans="2:39" x14ac:dyDescent="0.25">
+      <c r="E32">
+        <v>992</v>
+      </c>
+      <c r="F32" s="25"/>
+      <c r="G32" s="25"/>
+      <c r="H32" s="25"/>
+      <c r="I32" s="25"/>
+      <c r="J32" s="25"/>
+      <c r="K32" s="25"/>
+      <c r="L32" s="25"/>
+      <c r="M32" s="25"/>
+      <c r="N32" s="25"/>
+      <c r="O32" s="25"/>
+      <c r="P32" s="25"/>
+      <c r="Q32" s="25"/>
+      <c r="R32" s="25"/>
+      <c r="S32" s="25"/>
+      <c r="T32" s="25"/>
+      <c r="U32" s="25"/>
+      <c r="V32" s="25"/>
+      <c r="W32" s="25"/>
+      <c r="X32" s="25"/>
+      <c r="Y32" s="25"/>
+      <c r="Z32" s="25"/>
+      <c r="AA32" s="25"/>
+      <c r="AB32" s="25"/>
+      <c r="AC32" s="25"/>
+      <c r="AD32" s="25"/>
+      <c r="AE32" s="25"/>
+      <c r="AF32" s="25"/>
+      <c r="AG32" s="25"/>
+      <c r="AH32" s="25"/>
+      <c r="AI32" s="25"/>
+      <c r="AJ32" s="25"/>
+      <c r="AK32" s="25"/>
+      <c r="AL32">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="34" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="J34" s="23"/>
+      <c r="K34" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="L34" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="35" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="J35" s="79"/>
+      <c r="K35" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="L35" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="37" spans="2:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37" s="91"/>
+      <c r="G37" s="91"/>
+      <c r="H37" s="91"/>
+      <c r="I37" s="91"/>
+      <c r="J37" s="91"/>
+      <c r="K37" s="91"/>
+      <c r="L37" s="91"/>
+      <c r="M37" s="91"/>
+      <c r="N37" s="91"/>
+      <c r="O37" s="91"/>
+      <c r="P37" s="91"/>
+      <c r="Q37" s="91"/>
+      <c r="R37" s="91"/>
+      <c r="S37" s="91"/>
+      <c r="T37" s="91"/>
+      <c r="U37" s="91"/>
+      <c r="V37" s="91"/>
+      <c r="W37" s="91"/>
+      <c r="X37" s="91"/>
+      <c r="Y37" s="91"/>
+      <c r="Z37" s="91"/>
+      <c r="AA37" s="91"/>
+      <c r="AB37" s="91"/>
+      <c r="AC37" s="91"/>
+      <c r="AD37" s="91"/>
+      <c r="AE37" s="91"/>
+      <c r="AF37" s="91"/>
+      <c r="AG37" s="91"/>
+      <c r="AH37" s="91"/>
+      <c r="AI37" s="91"/>
+      <c r="AJ37" s="91"/>
+      <c r="AK37" s="91"/>
+      <c r="AL37">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="38" spans="2:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="135" t="s">
+        <v>161</v>
+      </c>
+      <c r="E38">
+        <v>32</v>
+      </c>
+      <c r="F38" s="91"/>
+      <c r="G38" s="91"/>
+      <c r="H38" s="91"/>
+      <c r="I38" s="91"/>
+      <c r="J38" s="91"/>
+      <c r="K38" s="91"/>
+      <c r="L38" s="91"/>
+      <c r="M38" s="91"/>
+      <c r="N38" s="91"/>
+      <c r="O38" s="91"/>
+      <c r="P38" s="91"/>
+      <c r="Q38" s="91"/>
+      <c r="R38" s="91"/>
+      <c r="S38" s="91"/>
+      <c r="T38" s="91"/>
+      <c r="U38" s="91"/>
+      <c r="V38" s="91"/>
+      <c r="W38" s="91"/>
+      <c r="X38" s="91"/>
+      <c r="Y38" s="91"/>
+      <c r="Z38" s="91"/>
+      <c r="AA38" s="91"/>
+      <c r="AB38" s="91"/>
+      <c r="AC38" s="91"/>
+      <c r="AD38" s="91"/>
+      <c r="AE38" s="91"/>
+      <c r="AF38" s="91"/>
+      <c r="AG38" s="91"/>
+      <c r="AH38" s="91"/>
+      <c r="AI38" s="91"/>
+      <c r="AJ38" s="91"/>
+      <c r="AK38" s="91"/>
+      <c r="AL38">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="B39" s="134" t="s">
+        <v>151</v>
+      </c>
+      <c r="E39">
+        <v>64</v>
+      </c>
+      <c r="F39" s="91"/>
+      <c r="G39" s="91"/>
+      <c r="H39" s="91"/>
+      <c r="I39" s="91"/>
+      <c r="J39" s="91"/>
+      <c r="K39" s="91"/>
+      <c r="L39" s="91"/>
+      <c r="M39" s="91"/>
+      <c r="N39" s="91"/>
+      <c r="O39" s="91"/>
+      <c r="P39" s="91"/>
+      <c r="Q39" s="80"/>
+      <c r="R39" s="115"/>
+      <c r="S39" s="52"/>
+      <c r="T39" s="119"/>
+      <c r="U39" s="52"/>
+      <c r="V39" s="119"/>
+      <c r="W39" s="118"/>
+      <c r="X39" s="117"/>
+      <c r="Y39" s="120"/>
+      <c r="Z39" s="118"/>
+      <c r="AA39" s="119"/>
+      <c r="AB39" s="52"/>
+      <c r="AC39" s="52"/>
+      <c r="AD39" s="119"/>
+      <c r="AE39" s="116"/>
+      <c r="AF39" s="67"/>
+      <c r="AG39" s="91"/>
+      <c r="AH39" s="91"/>
+      <c r="AI39" s="91"/>
+      <c r="AJ39" s="91"/>
+      <c r="AK39" s="91"/>
+      <c r="AL39">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="B40" s="132" t="s">
+        <v>150</v>
+      </c>
+      <c r="E40">
+        <v>96</v>
+      </c>
+      <c r="F40" s="91"/>
+      <c r="G40" s="91"/>
+      <c r="H40" s="91"/>
+      <c r="I40" s="91"/>
+      <c r="J40" s="91"/>
+      <c r="K40" s="91"/>
+      <c r="L40" s="91"/>
+      <c r="M40" s="92"/>
+      <c r="N40" s="92"/>
+      <c r="O40" s="92"/>
+      <c r="P40" s="92"/>
+      <c r="Q40" s="90"/>
+      <c r="R40" s="38"/>
+      <c r="S40" s="36"/>
+      <c r="T40" s="82"/>
+      <c r="U40" s="36"/>
+      <c r="V40" s="36"/>
+      <c r="W40" s="93"/>
+      <c r="X40" s="103"/>
+      <c r="Y40" s="103"/>
+      <c r="Z40" s="93"/>
+      <c r="AA40" s="36"/>
+      <c r="AB40" s="36"/>
+      <c r="AC40" s="36"/>
+      <c r="AD40" s="36"/>
+      <c r="AE40" s="42"/>
+      <c r="AF40" s="78"/>
+      <c r="AG40" s="91"/>
+      <c r="AH40" s="91"/>
+      <c r="AI40" s="91"/>
+      <c r="AJ40" s="91"/>
+      <c r="AK40" s="91"/>
+      <c r="AL40">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="41" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="B41" s="132"/>
+      <c r="E41">
+        <v>128</v>
+      </c>
+      <c r="F41" s="91"/>
+      <c r="G41" s="91"/>
+      <c r="H41" s="91"/>
+      <c r="I41" s="91"/>
+      <c r="J41" s="91"/>
+      <c r="K41" s="91"/>
+      <c r="L41" s="91"/>
+      <c r="M41" s="92"/>
+      <c r="N41" s="92"/>
+      <c r="O41" s="92"/>
+      <c r="P41" s="92"/>
+      <c r="Q41" s="75"/>
+      <c r="R41" s="39"/>
+      <c r="S41" s="43"/>
+      <c r="T41" s="94"/>
+      <c r="U41" s="95"/>
+      <c r="V41" s="125"/>
+      <c r="W41" s="125"/>
+      <c r="X41" s="94"/>
+      <c r="Y41" s="94"/>
+      <c r="Z41" s="125"/>
+      <c r="AA41" s="125"/>
+      <c r="AB41" s="94"/>
+      <c r="AC41" s="94"/>
+      <c r="AD41" s="29"/>
+      <c r="AE41" s="43"/>
+      <c r="AF41" s="78"/>
+      <c r="AG41" s="91"/>
+      <c r="AH41" s="91"/>
+      <c r="AI41" s="91"/>
+      <c r="AJ41" s="91"/>
+      <c r="AK41" s="91"/>
+      <c r="AL41">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="42" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="B42" s="132" t="s">
+        <v>153</v>
+      </c>
+      <c r="E42">
+        <v>160</v>
+      </c>
+      <c r="F42" s="91"/>
+      <c r="G42" s="91"/>
+      <c r="H42" s="91"/>
+      <c r="I42" s="91"/>
+      <c r="J42" s="91"/>
+      <c r="K42" s="91"/>
+      <c r="L42" s="91"/>
+      <c r="M42" s="92"/>
+      <c r="N42" s="92"/>
+      <c r="O42" s="92"/>
+      <c r="P42" s="92"/>
+      <c r="Q42" s="75"/>
+      <c r="R42" s="39"/>
+      <c r="S42" s="29"/>
+      <c r="T42" s="36"/>
+      <c r="U42" s="94"/>
+      <c r="V42" s="125"/>
+      <c r="W42" s="125"/>
+      <c r="X42" s="94"/>
+      <c r="Y42" s="94"/>
+      <c r="Z42" s="125"/>
+      <c r="AA42" s="125"/>
+      <c r="AB42" s="94"/>
+      <c r="AC42" s="29"/>
+      <c r="AD42" s="29"/>
+      <c r="AE42" s="43"/>
+      <c r="AF42" s="78"/>
+      <c r="AG42" s="91"/>
+      <c r="AH42" s="91"/>
+      <c r="AI42" s="91"/>
+      <c r="AJ42" s="91"/>
+      <c r="AK42" s="91"/>
+      <c r="AL42">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="43" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="B43" s="132" t="s">
+        <v>139</v>
+      </c>
+      <c r="E43">
+        <v>192</v>
+      </c>
+      <c r="F43" s="91"/>
+      <c r="G43" s="91"/>
+      <c r="H43" s="91"/>
+      <c r="I43" s="91"/>
+      <c r="J43" s="91"/>
+      <c r="K43" s="91"/>
+      <c r="L43" s="91"/>
+      <c r="M43" s="92"/>
+      <c r="N43" s="92"/>
+      <c r="O43" s="92"/>
+      <c r="P43" s="92"/>
+      <c r="Q43" s="75"/>
+      <c r="R43" s="39"/>
+      <c r="S43" s="29"/>
+      <c r="T43" s="29"/>
+      <c r="U43" s="29"/>
+      <c r="V43" s="94"/>
+      <c r="W43" s="94"/>
+      <c r="X43" s="94"/>
+      <c r="Y43" s="94"/>
+      <c r="Z43" s="94"/>
+      <c r="AA43" s="94"/>
+      <c r="AB43" s="29"/>
+      <c r="AC43" s="29"/>
+      <c r="AD43" s="29"/>
+      <c r="AE43" s="43"/>
+      <c r="AF43" s="78"/>
+      <c r="AG43" s="91"/>
+      <c r="AH43" s="91"/>
+      <c r="AI43" s="91"/>
+      <c r="AJ43" s="91"/>
+      <c r="AK43" s="91"/>
+      <c r="AL43">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="44" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="B44" s="132" t="s">
+        <v>140</v>
+      </c>
+      <c r="E44">
+        <v>224</v>
+      </c>
+      <c r="F44" s="91"/>
+      <c r="G44" s="91"/>
+      <c r="H44" s="91"/>
+      <c r="I44" s="91"/>
+      <c r="J44" s="91"/>
+      <c r="K44" s="91"/>
+      <c r="L44" s="91"/>
+      <c r="M44" s="92"/>
+      <c r="N44" s="92"/>
+      <c r="O44" s="92"/>
+      <c r="P44" s="92"/>
+      <c r="Q44" s="75"/>
+      <c r="R44" s="39"/>
+      <c r="S44" s="29"/>
+      <c r="T44" s="102"/>
+      <c r="U44" s="29"/>
+      <c r="V44" s="94"/>
+      <c r="W44" s="94"/>
+      <c r="X44" s="94"/>
+      <c r="Y44" s="94"/>
+      <c r="Z44" s="94"/>
+      <c r="AA44" s="94"/>
+      <c r="AB44" s="29"/>
+      <c r="AC44" s="102"/>
+      <c r="AD44" s="29"/>
+      <c r="AE44" s="43"/>
+      <c r="AF44" s="78"/>
+      <c r="AG44" s="91"/>
+      <c r="AH44" s="91"/>
+      <c r="AI44" s="91"/>
+      <c r="AJ44" s="91"/>
+      <c r="AK44" s="91"/>
+      <c r="AL44">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="45" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="B45" s="132"/>
+      <c r="E45">
+        <v>256</v>
+      </c>
+      <c r="F45" s="91"/>
+      <c r="G45" s="91"/>
+      <c r="H45" s="91"/>
+      <c r="I45" s="91"/>
+      <c r="J45" s="91"/>
+      <c r="K45" s="91"/>
+      <c r="L45" s="91"/>
+      <c r="M45" s="92"/>
+      <c r="N45" s="92"/>
+      <c r="O45" s="92"/>
+      <c r="P45" s="92"/>
+      <c r="Q45" s="75"/>
+      <c r="R45" s="39"/>
+      <c r="S45" s="29"/>
+      <c r="T45" s="102"/>
+      <c r="U45" s="94"/>
+      <c r="V45" s="131"/>
+      <c r="W45" s="131"/>
+      <c r="X45" s="94"/>
+      <c r="Y45" s="94"/>
+      <c r="Z45" s="131"/>
+      <c r="AA45" s="131"/>
+      <c r="AB45" s="94"/>
+      <c r="AC45" s="102"/>
+      <c r="AD45" s="29"/>
+      <c r="AE45" s="43"/>
+      <c r="AF45" s="78"/>
+      <c r="AG45" s="91"/>
+      <c r="AH45" s="91"/>
+      <c r="AI45" s="91"/>
+      <c r="AJ45" s="91"/>
+      <c r="AK45" s="91"/>
+      <c r="AL45">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="46" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="B46" s="132" t="s">
+        <v>152</v>
+      </c>
+      <c r="E46">
+        <v>288</v>
+      </c>
+      <c r="F46" s="91"/>
+      <c r="G46" s="91"/>
+      <c r="H46" s="91"/>
+      <c r="I46" s="91"/>
+      <c r="J46" s="91"/>
+      <c r="K46" s="91"/>
+      <c r="L46" s="91"/>
+      <c r="M46" s="92"/>
+      <c r="N46" s="92"/>
+      <c r="O46" s="92"/>
+      <c r="P46" s="92"/>
+      <c r="Q46" s="75"/>
+      <c r="R46" s="39"/>
+      <c r="S46" s="94"/>
+      <c r="T46" s="94"/>
+      <c r="U46" s="94"/>
+      <c r="V46" s="131"/>
+      <c r="W46" s="131"/>
+      <c r="X46" s="94"/>
+      <c r="Y46" s="94"/>
+      <c r="Z46" s="131"/>
+      <c r="AA46" s="131"/>
+      <c r="AB46" s="94"/>
+      <c r="AC46" s="94"/>
+      <c r="AD46" s="94"/>
+      <c r="AE46" s="43"/>
+      <c r="AF46" s="78"/>
+      <c r="AG46" s="91"/>
+      <c r="AH46" s="91"/>
+      <c r="AI46" s="91"/>
+      <c r="AJ46" s="91"/>
+      <c r="AK46" s="91"/>
+      <c r="AL46">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="47" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="B47" s="132" t="s">
+        <v>154</v>
+      </c>
+      <c r="E47">
+        <v>320</v>
+      </c>
+      <c r="F47" s="91"/>
+      <c r="G47" s="91"/>
+      <c r="H47" s="91"/>
+      <c r="I47" s="91"/>
+      <c r="J47" s="91"/>
+      <c r="K47" s="91"/>
+      <c r="L47" s="91"/>
+      <c r="M47" s="92"/>
+      <c r="N47" s="92"/>
+      <c r="O47" s="92"/>
+      <c r="P47" s="92"/>
+      <c r="Q47" s="96"/>
+      <c r="R47" s="95"/>
+      <c r="S47" s="94"/>
+      <c r="T47" s="94"/>
+      <c r="U47" s="94"/>
+      <c r="V47" s="131"/>
+      <c r="W47" s="131"/>
+      <c r="X47" s="131"/>
+      <c r="Y47" s="131"/>
+      <c r="Z47" s="131"/>
+      <c r="AA47" s="131"/>
+      <c r="AB47" s="94"/>
+      <c r="AC47" s="94"/>
+      <c r="AD47" s="94"/>
+      <c r="AE47" s="97"/>
+      <c r="AF47" s="98"/>
+      <c r="AG47" s="91"/>
+      <c r="AH47" s="91"/>
+      <c r="AI47" s="91"/>
+      <c r="AJ47" s="91"/>
+      <c r="AK47" s="91"/>
+      <c r="AL47">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="48" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="B48" s="132" t="s">
+        <v>155</v>
+      </c>
+      <c r="E48">
+        <v>352</v>
+      </c>
+      <c r="F48" s="91"/>
+      <c r="G48" s="91"/>
+      <c r="H48" s="91"/>
+      <c r="I48" s="91"/>
+      <c r="J48" s="91"/>
+      <c r="K48" s="91"/>
+      <c r="L48" s="91"/>
+      <c r="M48" s="91"/>
+      <c r="N48" s="91"/>
+      <c r="O48" s="91"/>
+      <c r="P48" s="91"/>
+      <c r="Q48" s="104"/>
+      <c r="R48" s="95"/>
+      <c r="S48" s="94"/>
+      <c r="T48" s="94"/>
+      <c r="U48" s="94"/>
+      <c r="V48" s="131"/>
+      <c r="W48" s="131"/>
+      <c r="X48" s="131"/>
+      <c r="Y48" s="131"/>
+      <c r="Z48" s="131"/>
+      <c r="AA48" s="131"/>
+      <c r="AB48" s="94"/>
+      <c r="AC48" s="94"/>
+      <c r="AD48" s="94"/>
+      <c r="AE48" s="97"/>
+      <c r="AF48" s="105"/>
+      <c r="AG48" s="91"/>
+      <c r="AH48" s="91"/>
+      <c r="AI48" s="91"/>
+      <c r="AJ48" s="91"/>
+      <c r="AK48" s="91"/>
+      <c r="AL48">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="49" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="B49" s="132" t="s">
+        <v>142</v>
+      </c>
+      <c r="E49">
+        <v>384</v>
+      </c>
+      <c r="F49" s="91"/>
+      <c r="G49" s="91"/>
+      <c r="H49" s="91"/>
+      <c r="I49" s="91"/>
+      <c r="J49" s="91"/>
+      <c r="K49" s="91"/>
+      <c r="L49" s="91"/>
+      <c r="M49" s="91"/>
+      <c r="N49" s="91"/>
+      <c r="O49" s="91"/>
+      <c r="P49" s="91"/>
+      <c r="Q49" s="104"/>
+      <c r="R49" s="95"/>
+      <c r="S49" s="125"/>
+      <c r="T49" s="94"/>
+      <c r="U49" s="94"/>
+      <c r="V49" s="102"/>
+      <c r="W49" s="125"/>
+      <c r="X49" s="102"/>
+      <c r="Y49" s="102"/>
+      <c r="Z49" s="125"/>
+      <c r="AA49" s="102"/>
+      <c r="AB49" s="94"/>
+      <c r="AC49" s="94"/>
+      <c r="AD49" s="125"/>
+      <c r="AE49" s="97"/>
+      <c r="AF49" s="105"/>
+      <c r="AG49" s="91"/>
+      <c r="AH49" s="91"/>
+      <c r="AI49" s="91"/>
+      <c r="AJ49" s="91"/>
+      <c r="AK49" s="91"/>
+      <c r="AL49">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="50" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="B50" s="132"/>
+      <c r="E50">
+        <v>416</v>
+      </c>
+      <c r="F50" s="91"/>
+      <c r="G50" s="91"/>
+      <c r="H50" s="91"/>
+      <c r="I50" s="91"/>
+      <c r="J50" s="91"/>
+      <c r="K50" s="91"/>
+      <c r="L50" s="91"/>
+      <c r="M50" s="91"/>
+      <c r="N50" s="91"/>
+      <c r="O50" s="91"/>
+      <c r="P50" s="91"/>
+      <c r="Q50" s="96"/>
+      <c r="R50" s="95"/>
+      <c r="S50" s="125"/>
+      <c r="T50" s="94"/>
+      <c r="U50" s="102"/>
+      <c r="V50" s="102"/>
+      <c r="W50" s="125"/>
+      <c r="X50" s="102"/>
+      <c r="Y50" s="102"/>
+      <c r="Z50" s="125"/>
+      <c r="AA50" s="102"/>
+      <c r="AB50" s="102"/>
+      <c r="AC50" s="94"/>
+      <c r="AD50" s="125"/>
+      <c r="AE50" s="97"/>
+      <c r="AF50" s="98"/>
+      <c r="AG50" s="91"/>
+      <c r="AH50" s="91"/>
+      <c r="AI50" s="91"/>
+      <c r="AJ50" s="91"/>
+      <c r="AK50" s="91"/>
+      <c r="AL50">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="51" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="B51" s="132" t="s">
+        <v>143</v>
+      </c>
+      <c r="E51">
+        <v>448</v>
+      </c>
+      <c r="F51" s="91"/>
+      <c r="G51" s="91"/>
+      <c r="H51" s="91"/>
+      <c r="I51" s="91"/>
+      <c r="J51" s="91"/>
+      <c r="K51" s="92"/>
+      <c r="L51" s="92"/>
+      <c r="M51" s="92"/>
+      <c r="N51" s="92"/>
+      <c r="O51" s="92"/>
+      <c r="P51" s="92"/>
+      <c r="Q51" s="96"/>
+      <c r="R51" s="126"/>
+      <c r="S51" s="94"/>
+      <c r="T51" s="94"/>
+      <c r="U51" s="102"/>
+      <c r="V51" s="102"/>
+      <c r="W51" s="102"/>
+      <c r="X51" s="102"/>
+      <c r="Y51" s="102"/>
+      <c r="Z51" s="102"/>
+      <c r="AA51" s="102"/>
+      <c r="AB51" s="102"/>
+      <c r="AC51" s="94"/>
+      <c r="AD51" s="94"/>
+      <c r="AE51" s="128"/>
+      <c r="AF51" s="98"/>
+      <c r="AG51" s="91"/>
+      <c r="AH51" s="91"/>
+      <c r="AI51" s="91"/>
+      <c r="AJ51" s="91"/>
+      <c r="AK51" s="91"/>
+      <c r="AL51">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="52" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="B52" s="132" t="s">
+        <v>156</v>
+      </c>
+      <c r="E52">
+        <v>480</v>
+      </c>
+      <c r="F52" s="91"/>
+      <c r="G52" s="91"/>
+      <c r="H52" s="91"/>
+      <c r="I52" s="91"/>
+      <c r="J52" s="91"/>
+      <c r="K52" s="92"/>
+      <c r="L52" s="92"/>
+      <c r="M52" s="92"/>
+      <c r="N52" s="92"/>
+      <c r="O52" s="92"/>
+      <c r="P52" s="92"/>
+      <c r="Q52" s="96"/>
+      <c r="R52" s="126"/>
+      <c r="S52" s="125"/>
+      <c r="T52" s="94"/>
+      <c r="U52" s="102"/>
+      <c r="V52" s="102"/>
+      <c r="W52" s="102"/>
+      <c r="X52" s="102"/>
+      <c r="Y52" s="102"/>
+      <c r="Z52" s="102"/>
+      <c r="AA52" s="102"/>
+      <c r="AB52" s="102"/>
+      <c r="AC52" s="94"/>
+      <c r="AD52" s="125"/>
+      <c r="AE52" s="128"/>
+      <c r="AF52" s="98"/>
+      <c r="AG52" s="91"/>
+      <c r="AH52" s="91"/>
+      <c r="AI52" s="91"/>
+      <c r="AJ52" s="91"/>
+      <c r="AK52" s="91"/>
+      <c r="AL52">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="53" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="B53" s="132" t="s">
+        <v>157</v>
+      </c>
+      <c r="E53">
+        <v>512</v>
+      </c>
+      <c r="F53" s="91"/>
+      <c r="G53" s="91"/>
+      <c r="H53" s="91"/>
+      <c r="I53" s="91"/>
+      <c r="J53" s="91"/>
+      <c r="K53" s="92"/>
+      <c r="L53" s="92"/>
+      <c r="M53" s="92"/>
+      <c r="N53" s="92"/>
+      <c r="O53" s="92"/>
+      <c r="P53" s="92"/>
+      <c r="Q53" s="100"/>
+      <c r="R53" s="127"/>
+      <c r="S53" s="130"/>
+      <c r="T53" s="99"/>
+      <c r="U53" s="107"/>
+      <c r="V53" s="107"/>
+      <c r="W53" s="107"/>
+      <c r="X53" s="107"/>
+      <c r="Y53" s="107"/>
+      <c r="Z53" s="107"/>
+      <c r="AA53" s="107"/>
+      <c r="AB53" s="107"/>
+      <c r="AC53" s="99"/>
+      <c r="AD53" s="130"/>
+      <c r="AE53" s="129"/>
+      <c r="AF53" s="101"/>
+      <c r="AG53" s="91"/>
+      <c r="AH53" s="91"/>
+      <c r="AI53" s="91"/>
+      <c r="AJ53" s="91"/>
+      <c r="AK53" s="91"/>
+      <c r="AL53">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="54" spans="2:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B54" s="132" t="s">
+        <v>158</v>
+      </c>
+      <c r="E54">
+        <v>544</v>
+      </c>
+      <c r="F54" s="91"/>
+      <c r="G54" s="91"/>
+      <c r="H54" s="91"/>
+      <c r="I54" s="91"/>
+      <c r="J54" s="91"/>
+      <c r="K54" s="92"/>
+      <c r="L54" s="92"/>
+      <c r="M54" s="92"/>
+      <c r="N54" s="92"/>
+      <c r="O54" s="92"/>
+      <c r="P54" s="92"/>
+      <c r="Q54" s="106"/>
+      <c r="R54" s="109"/>
+      <c r="S54" s="110"/>
+      <c r="T54" s="111"/>
+      <c r="U54" s="111"/>
+      <c r="V54" s="111"/>
+      <c r="W54" s="112"/>
+      <c r="X54" s="112"/>
+      <c r="Y54" s="112"/>
+      <c r="Z54" s="112"/>
+      <c r="AA54" s="112"/>
+      <c r="AB54" s="112"/>
+      <c r="AC54" s="111"/>
+      <c r="AD54" s="110"/>
+      <c r="AE54" s="113"/>
+      <c r="AF54" s="108"/>
+      <c r="AG54" s="91"/>
+      <c r="AH54" s="91"/>
+      <c r="AI54" s="91"/>
+      <c r="AJ54" s="91"/>
+      <c r="AK54" s="91"/>
+      <c r="AL54">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="55" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="B55" s="132" t="s">
+        <v>160</v>
+      </c>
+      <c r="E55">
+        <v>576</v>
+      </c>
+      <c r="F55" s="91"/>
+      <c r="G55" s="91"/>
+      <c r="H55" s="91"/>
+      <c r="I55" s="91"/>
+      <c r="J55" s="91"/>
+      <c r="K55" s="92"/>
+      <c r="L55" s="92"/>
+      <c r="M55" s="92"/>
+      <c r="N55" s="92"/>
+      <c r="O55" s="92"/>
+      <c r="P55" s="92"/>
+      <c r="Q55" s="92"/>
+      <c r="R55" s="92"/>
+      <c r="S55" s="92"/>
+      <c r="T55" s="92"/>
+      <c r="U55" s="92"/>
+      <c r="V55" s="92"/>
+      <c r="W55" s="92"/>
+      <c r="X55" s="92"/>
+      <c r="Y55" s="92"/>
+      <c r="Z55" s="92"/>
+      <c r="AA55" s="91"/>
+      <c r="AB55" s="91"/>
+      <c r="AC55" s="91"/>
+      <c r="AD55" s="91"/>
+      <c r="AE55" s="91"/>
+      <c r="AF55" s="91"/>
+      <c r="AG55" s="91"/>
+      <c r="AH55" s="91"/>
+      <c r="AI55" s="91"/>
+      <c r="AJ55" s="91"/>
+      <c r="AK55" s="91"/>
+      <c r="AL55">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="56" spans="2:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="133" t="s">
+        <v>147</v>
+      </c>
+      <c r="E56">
+        <v>608</v>
+      </c>
+      <c r="F56" s="91"/>
+      <c r="G56" s="91"/>
+      <c r="H56" s="91"/>
+      <c r="I56" s="91"/>
+      <c r="J56" s="91"/>
+      <c r="K56" s="92"/>
+      <c r="L56" s="92"/>
+      <c r="M56" s="92"/>
+      <c r="N56" s="92"/>
+      <c r="O56" s="92"/>
+      <c r="P56" s="92"/>
+      <c r="Q56" s="92"/>
+      <c r="R56" s="92"/>
+      <c r="S56" s="92"/>
+      <c r="T56" s="92"/>
+      <c r="U56" s="92"/>
+      <c r="V56" s="92"/>
+      <c r="W56" s="92"/>
+      <c r="X56" s="92"/>
+      <c r="Y56" s="92"/>
+      <c r="Z56" s="92"/>
+      <c r="AA56" s="91"/>
+      <c r="AB56" s="91"/>
+      <c r="AC56" s="91"/>
+      <c r="AD56" s="91"/>
+      <c r="AE56" s="91"/>
+      <c r="AF56" s="91"/>
+      <c r="AG56" s="91"/>
+      <c r="AH56" s="91"/>
+      <c r="AI56" s="91"/>
+      <c r="AJ56" s="91"/>
+      <c r="AK56" s="91"/>
+      <c r="AL56">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="57" spans="2:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E57">
+        <v>640</v>
+      </c>
+      <c r="F57" s="91"/>
+      <c r="G57" s="91"/>
+      <c r="H57" s="91"/>
+      <c r="I57" s="91"/>
+      <c r="J57" s="91"/>
+      <c r="K57" s="92"/>
+      <c r="L57" s="92"/>
+      <c r="M57" s="92"/>
+      <c r="N57" s="92"/>
+      <c r="O57" s="92"/>
+      <c r="P57" s="92"/>
+      <c r="Q57" s="92"/>
+      <c r="R57" s="92"/>
+      <c r="S57" s="92"/>
+      <c r="T57" s="92"/>
+      <c r="U57" s="92"/>
+      <c r="V57" s="92"/>
+      <c r="W57" s="92"/>
+      <c r="X57" s="92"/>
+      <c r="Y57" s="92"/>
+      <c r="Z57" s="92"/>
+      <c r="AA57" s="91"/>
+      <c r="AB57" s="91"/>
+      <c r="AC57" s="91"/>
+      <c r="AD57" s="91"/>
+      <c r="AE57" s="91"/>
+      <c r="AF57" s="91"/>
+      <c r="AG57" s="91"/>
+      <c r="AH57" s="91"/>
+      <c r="AI57" s="91"/>
+      <c r="AJ57" s="91"/>
+      <c r="AK57" s="91"/>
+      <c r="AL57">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="58" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="E58">
+        <v>672</v>
+      </c>
+      <c r="F58" s="91"/>
+      <c r="G58" s="91"/>
+      <c r="H58" s="91"/>
+      <c r="I58" s="91"/>
+      <c r="J58" s="91"/>
+      <c r="K58" s="92"/>
+      <c r="L58" s="92"/>
+      <c r="M58" s="92"/>
+      <c r="N58" s="92"/>
+      <c r="O58" s="92"/>
+      <c r="P58" s="92"/>
+      <c r="Q58" s="92"/>
+      <c r="R58" s="92"/>
+      <c r="S58" s="92"/>
+      <c r="T58" s="92"/>
+      <c r="U58" s="92"/>
+      <c r="V58" s="92"/>
+      <c r="W58" s="51"/>
+      <c r="X58" s="52"/>
+      <c r="Y58" s="52"/>
+      <c r="Z58" s="65"/>
+      <c r="AA58" s="52"/>
+      <c r="AB58" s="52"/>
+      <c r="AC58" s="52"/>
+      <c r="AD58" s="53"/>
+      <c r="AE58" s="91"/>
+      <c r="AF58" s="91"/>
+      <c r="AG58" s="91"/>
+      <c r="AH58" s="91"/>
+      <c r="AI58" s="91"/>
+      <c r="AJ58" s="91"/>
+      <c r="AK58" s="91"/>
+      <c r="AL58">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="59" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="E59">
+        <v>704</v>
+      </c>
+      <c r="F59" s="91"/>
+      <c r="G59" s="91"/>
+      <c r="H59" s="91"/>
+      <c r="I59" s="91"/>
+      <c r="J59" s="91"/>
+      <c r="K59" s="92"/>
+      <c r="L59" s="92"/>
+      <c r="M59" s="92"/>
+      <c r="N59" s="92"/>
+      <c r="O59" s="92"/>
+      <c r="P59" s="92"/>
+      <c r="Q59" s="92"/>
+      <c r="R59" s="92"/>
+      <c r="S59" s="92"/>
+      <c r="T59" s="92"/>
+      <c r="U59" s="92"/>
+      <c r="V59" s="92"/>
+      <c r="W59" s="54"/>
+      <c r="X59" s="29"/>
+      <c r="Y59" s="63"/>
+      <c r="Z59" s="121"/>
+      <c r="AA59" s="39"/>
+      <c r="AB59" s="29"/>
+      <c r="AC59" s="29"/>
+      <c r="AD59" s="55"/>
+      <c r="AE59" s="92"/>
+      <c r="AF59" s="91"/>
+      <c r="AG59" s="91"/>
+      <c r="AH59" s="91"/>
+      <c r="AI59" s="91"/>
+      <c r="AJ59" s="91"/>
+      <c r="AK59" s="91"/>
+      <c r="AL59">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="60" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="E60">
+        <v>736</v>
+      </c>
+      <c r="F60" s="91"/>
+      <c r="G60" s="91"/>
+      <c r="H60" s="91"/>
+      <c r="I60" s="91"/>
+      <c r="J60" s="91"/>
+      <c r="K60" s="92"/>
+      <c r="L60" s="92"/>
+      <c r="M60" s="92"/>
+      <c r="N60" s="92"/>
+      <c r="O60" s="92"/>
+      <c r="P60" s="92"/>
+      <c r="Q60" s="92"/>
+      <c r="R60" s="92"/>
+      <c r="S60" s="92"/>
+      <c r="T60" s="92"/>
+      <c r="U60" s="92"/>
+      <c r="V60" s="92"/>
+      <c r="W60" s="54"/>
+      <c r="X60" s="29"/>
+      <c r="Y60" s="29"/>
+      <c r="Z60" s="124"/>
+      <c r="AA60" s="122"/>
+      <c r="AB60" s="29"/>
+      <c r="AC60" s="29"/>
+      <c r="AD60" s="55"/>
+      <c r="AE60" s="92"/>
+      <c r="AF60" s="91"/>
+      <c r="AG60" s="91"/>
+      <c r="AH60" s="91"/>
+      <c r="AI60" s="91"/>
+      <c r="AJ60" s="91"/>
+      <c r="AK60" s="91"/>
+      <c r="AL60">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="61" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="E61">
+        <v>768</v>
+      </c>
+      <c r="F61" s="91"/>
+      <c r="G61" s="91"/>
+      <c r="H61" s="91"/>
+      <c r="I61" s="91"/>
+      <c r="J61" s="91"/>
+      <c r="K61" s="92"/>
+      <c r="L61" s="92"/>
+      <c r="M61" s="92"/>
+      <c r="N61" s="92"/>
+      <c r="O61" s="92"/>
+      <c r="P61" s="92"/>
+      <c r="Q61" s="92"/>
+      <c r="R61" s="92"/>
+      <c r="S61" s="92"/>
+      <c r="T61" s="92"/>
+      <c r="U61" s="92"/>
+      <c r="V61" s="92"/>
+      <c r="W61" s="54"/>
+      <c r="X61" s="29"/>
+      <c r="Y61" s="29"/>
+      <c r="Z61" s="122"/>
+      <c r="AA61" s="34"/>
+      <c r="AB61" s="29"/>
+      <c r="AC61" s="29"/>
+      <c r="AD61" s="55"/>
+      <c r="AE61" s="92"/>
+      <c r="AF61" s="91"/>
+      <c r="AG61" s="91"/>
+      <c r="AH61" s="91"/>
+      <c r="AI61" s="91"/>
+      <c r="AJ61" s="91"/>
+      <c r="AK61" s="91"/>
+      <c r="AL61">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="62" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="E62">
+        <v>800</v>
+      </c>
+      <c r="F62" s="91"/>
+      <c r="G62" s="91"/>
+      <c r="H62" s="91"/>
+      <c r="I62" s="91"/>
+      <c r="J62" s="91"/>
+      <c r="K62" s="92"/>
+      <c r="L62" s="92"/>
+      <c r="M62" s="92"/>
+      <c r="N62" s="92"/>
+      <c r="O62" s="92"/>
+      <c r="P62" s="92"/>
+      <c r="Q62" s="92"/>
+      <c r="R62" s="92"/>
+      <c r="S62" s="92"/>
+      <c r="T62" s="92"/>
+      <c r="U62" s="92"/>
+      <c r="V62" s="92"/>
+      <c r="W62" s="54"/>
+      <c r="X62" s="29"/>
+      <c r="Y62" s="29"/>
+      <c r="Z62" s="122"/>
+      <c r="AA62" s="122"/>
+      <c r="AB62" s="29"/>
+      <c r="AC62" s="29"/>
+      <c r="AD62" s="55"/>
+      <c r="AE62" s="92"/>
+      <c r="AF62" s="91"/>
+      <c r="AG62" s="91"/>
+      <c r="AH62" s="91"/>
+      <c r="AI62" s="91"/>
+      <c r="AJ62" s="91"/>
+      <c r="AK62" s="91"/>
+      <c r="AL62">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="63" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="E63">
+        <v>832</v>
+      </c>
+      <c r="F63" s="91"/>
+      <c r="G63" s="91"/>
+      <c r="H63" s="91"/>
+      <c r="I63" s="91"/>
+      <c r="J63" s="91"/>
+      <c r="K63" s="92"/>
+      <c r="L63" s="92"/>
+      <c r="M63" s="92"/>
+      <c r="N63" s="92"/>
+      <c r="O63" s="92"/>
+      <c r="P63" s="92"/>
+      <c r="Q63" s="92"/>
+      <c r="R63" s="92"/>
+      <c r="S63" s="92"/>
+      <c r="T63" s="92"/>
+      <c r="U63" s="92"/>
+      <c r="V63" s="92"/>
+      <c r="W63" s="54"/>
+      <c r="X63" s="29"/>
+      <c r="Y63" s="29"/>
+      <c r="Z63" s="122"/>
+      <c r="AA63" s="123"/>
+      <c r="AB63" s="29"/>
+      <c r="AC63" s="29"/>
+      <c r="AD63" s="55"/>
+      <c r="AE63" s="92"/>
+      <c r="AF63" s="91"/>
+      <c r="AG63" s="91"/>
+      <c r="AH63" s="91"/>
+      <c r="AI63" s="91"/>
+      <c r="AJ63" s="91"/>
+      <c r="AK63" s="91"/>
+      <c r="AL63">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="64" spans="2:38" x14ac:dyDescent="0.25">
+      <c r="E64">
+        <v>864</v>
+      </c>
+      <c r="F64" s="91"/>
+      <c r="G64" s="91"/>
+      <c r="H64" s="91"/>
+      <c r="I64" s="91"/>
+      <c r="J64" s="91"/>
+      <c r="K64" s="92"/>
+      <c r="L64" s="92"/>
+      <c r="M64" s="92"/>
+      <c r="N64" s="92"/>
+      <c r="O64" s="92"/>
+      <c r="P64" s="92"/>
+      <c r="Q64" s="92"/>
+      <c r="R64" s="92"/>
+      <c r="S64" s="92"/>
+      <c r="T64" s="92"/>
+      <c r="U64" s="92"/>
+      <c r="V64" s="92"/>
+      <c r="W64" s="54"/>
+      <c r="X64" s="29"/>
+      <c r="Y64" s="29"/>
+      <c r="Z64" s="63"/>
+      <c r="AA64" s="121"/>
+      <c r="AB64" s="39"/>
+      <c r="AC64" s="29"/>
+      <c r="AD64" s="55"/>
+      <c r="AE64" s="92"/>
+      <c r="AF64" s="91"/>
+      <c r="AG64" s="91"/>
+      <c r="AH64" s="91"/>
+      <c r="AI64" s="91"/>
+      <c r="AJ64" s="91"/>
+      <c r="AK64" s="91"/>
+      <c r="AL64">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="65" spans="5:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E65">
+        <v>896</v>
+      </c>
+      <c r="F65" s="91"/>
+      <c r="G65" s="91"/>
+      <c r="H65" s="91"/>
+      <c r="I65" s="91"/>
+      <c r="J65" s="91"/>
+      <c r="K65" s="92"/>
+      <c r="L65" s="92"/>
+      <c r="M65" s="92"/>
+      <c r="N65" s="92"/>
+      <c r="O65" s="92"/>
+      <c r="P65" s="92"/>
+      <c r="Q65" s="92"/>
+      <c r="R65" s="92"/>
+      <c r="S65" s="92"/>
+      <c r="T65" s="92"/>
+      <c r="U65" s="92"/>
+      <c r="V65" s="92"/>
+      <c r="W65" s="56"/>
+      <c r="X65" s="57"/>
+      <c r="Y65" s="57"/>
+      <c r="Z65" s="57"/>
+      <c r="AA65" s="59"/>
+      <c r="AB65" s="57"/>
+      <c r="AC65" s="57"/>
+      <c r="AD65" s="58"/>
+      <c r="AE65" s="92"/>
+      <c r="AF65" s="91"/>
+      <c r="AG65" s="91"/>
+      <c r="AH65" s="91"/>
+      <c r="AI65" s="91"/>
+      <c r="AJ65" s="91"/>
+      <c r="AK65" s="91"/>
+      <c r="AL65">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="66" spans="5:38" x14ac:dyDescent="0.25">
+      <c r="E66">
+        <v>928</v>
+      </c>
+      <c r="F66" s="91"/>
+      <c r="G66" s="91"/>
+      <c r="H66" s="91"/>
+      <c r="I66" s="91"/>
+      <c r="J66" s="91"/>
+      <c r="K66" s="92"/>
+      <c r="L66" s="92"/>
+      <c r="M66" s="92"/>
+      <c r="N66" s="92"/>
+      <c r="O66" s="92"/>
+      <c r="P66" s="92"/>
+      <c r="Q66" s="92"/>
+      <c r="R66" s="92"/>
+      <c r="S66" s="92"/>
+      <c r="T66" s="92"/>
+      <c r="U66" s="92"/>
+      <c r="V66" s="92"/>
+      <c r="W66" s="92"/>
+      <c r="X66" s="92"/>
+      <c r="Y66" s="92"/>
+      <c r="Z66" s="92"/>
+      <c r="AA66" s="92"/>
+      <c r="AB66" s="92"/>
+      <c r="AC66" s="92"/>
+      <c r="AD66" s="92"/>
+      <c r="AE66" s="92"/>
+      <c r="AF66" s="91"/>
+      <c r="AG66" s="91"/>
+      <c r="AH66" s="91"/>
+      <c r="AI66" s="91"/>
+      <c r="AJ66" s="91"/>
+      <c r="AK66" s="91"/>
+      <c r="AL66">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="67" spans="5:38" x14ac:dyDescent="0.25">
+      <c r="E67">
+        <v>960</v>
+      </c>
+      <c r="F67" s="91"/>
+      <c r="G67" s="91"/>
+      <c r="H67" s="91"/>
+      <c r="I67" s="91"/>
+      <c r="J67" s="91"/>
+      <c r="K67" s="91"/>
+      <c r="L67" s="91"/>
+      <c r="M67" s="91"/>
+      <c r="N67" s="91"/>
+      <c r="O67" s="91"/>
+      <c r="P67" s="91"/>
+      <c r="Q67" s="91"/>
+      <c r="R67" s="91"/>
+      <c r="S67" s="91"/>
+      <c r="T67" s="91"/>
+      <c r="U67" s="91"/>
+      <c r="V67" s="91"/>
+      <c r="W67" s="91"/>
+      <c r="X67" s="91"/>
+      <c r="Y67" s="91"/>
+      <c r="Z67" s="91"/>
+      <c r="AA67" s="91"/>
+      <c r="AB67" s="91"/>
+      <c r="AC67" s="91"/>
+      <c r="AD67" s="91"/>
+      <c r="AE67" s="91"/>
+      <c r="AF67" s="91"/>
+      <c r="AG67" s="91"/>
+      <c r="AH67" s="91"/>
+      <c r="AI67" s="91"/>
+      <c r="AJ67" s="91"/>
+      <c r="AK67" s="91"/>
+      <c r="AL67">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="68" spans="5:38" x14ac:dyDescent="0.25">
+      <c r="E68">
+        <v>992</v>
+      </c>
+      <c r="F68" s="91"/>
+      <c r="G68" s="91"/>
+      <c r="H68" s="91"/>
+      <c r="I68" s="91"/>
+      <c r="J68" s="91"/>
+      <c r="K68" s="91"/>
+      <c r="L68" s="91"/>
+      <c r="M68" s="91"/>
+      <c r="N68" s="91"/>
+      <c r="O68" s="91"/>
+      <c r="P68" s="91"/>
+      <c r="Q68" s="91"/>
+      <c r="R68" s="91"/>
+      <c r="S68" s="91"/>
+      <c r="T68" s="91"/>
+      <c r="U68" s="91"/>
+      <c r="V68" s="91"/>
+      <c r="W68" s="91"/>
+      <c r="X68" s="91"/>
+      <c r="Y68" s="91"/>
+      <c r="Z68" s="91"/>
+      <c r="AA68" s="91"/>
+      <c r="AB68" s="91"/>
+      <c r="AC68" s="91"/>
+      <c r="AD68" s="91"/>
+      <c r="AE68" s="91"/>
+      <c r="AF68" s="91"/>
+      <c r="AG68" s="91"/>
+      <c r="AH68" s="91"/>
+      <c r="AI68" s="91"/>
+      <c r="AJ68" s="91"/>
+      <c r="AK68" s="91"/>
+      <c r="AL68">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="83" spans="39:39" x14ac:dyDescent="0.25">
+      <c r="AM83" s="114"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>